<commit_message>
Added OOI bar codes and corrected reference designators
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP01CNSM_00004.xlsx
+++ b/deployment/Omaha_Cal_Info_CP01CNSM_00004.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14740" yWindow="800" windowWidth="20740" windowHeight="11760" tabRatio="766" activeTab="1"/>
+    <workbookView xWindow="90" yWindow="1395" windowWidth="20730" windowHeight="11760" tabRatio="766" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -19,7 +24,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1803,7 +1808,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1862,7 +1867,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1897,7 +1902,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2110,26 +2115,26 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="61" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" style="61" customWidth="1"/>
     <col min="2" max="2" width="16" style="61" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="61" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" style="61" customWidth="1"/>
-    <col min="5" max="5" width="11.5" style="62" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" style="63" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="62" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="61" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="61" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" style="61" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="61" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.6640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" style="61" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="62" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="62" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="61" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" style="61" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" style="61" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" style="61" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="61"/>
+    <col min="14" max="14" width="12.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="58" customFormat="1" ht="28">
+    <row r="1" spans="1:14" s="58" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="53" t="s">
         <v>151</v>
       </c>
@@ -2167,7 +2172,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="61" t="s">
         <v>152</v>
       </c>
@@ -2209,8 +2214,8 @@
         <v>-70.778433333333339</v>
       </c>
     </row>
-    <row r="4" spans="1:14" customFormat="1"/>
-    <row r="5" spans="1:14" customFormat="1"/>
+    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2227,30 +2232,30 @@
   <dimension ref="A1:V383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="44" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="44" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="45" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="45.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.33203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="1"/>
-    <col min="11" max="11" width="4.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="45" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="8" customWidth="1"/>
+    <col min="10" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="4.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="1"/>
+    <col min="15" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="28">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2283,7 +2288,7 @@
       <c r="L1" s="36"/>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C2" s="18"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -2291,7 +2296,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -2314,7 +2319,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="44" customFormat="1">
+    <row r="4" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="42"/>
       <c r="B4" s="42"/>
       <c r="C4" s="17"/>
@@ -2324,7 +2329,7 @@
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
     </row>
-    <row r="5" spans="1:18" s="73" customFormat="1">
+    <row r="5" spans="1:18" s="73" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="89" t="s">
         <v>114</v>
       </c>
@@ -2349,7 +2354,7 @@
       <c r="M5" s="44"/>
       <c r="R5" s="44"/>
     </row>
-    <row r="6" spans="1:18" s="73" customFormat="1">
+    <row r="6" spans="1:18" s="73" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="89" t="s">
         <v>115</v>
       </c>
@@ -2374,12 +2379,12 @@
       <c r="M6" s="44"/>
       <c r="R6" s="44"/>
     </row>
-    <row r="7" spans="1:18" s="44" customFormat="1">
+    <row r="7" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C7" s="42"/>
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2408,7 +2413,7 @@
       <c r="M8" s="44"/>
       <c r="R8" s="44"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2437,7 +2442,7 @@
       <c r="M9" s="44"/>
       <c r="R9" s="44"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -2466,7 +2471,7 @@
       <c r="M10" s="44"/>
       <c r="R10" s="44"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -2495,7 +2500,7 @@
       <c r="M11" s="44"/>
       <c r="R11" s="44"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -2524,7 +2529,7 @@
       <c r="M12" s="44"/>
       <c r="R12" s="44"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -2553,7 +2558,7 @@
       <c r="M13" s="44"/>
       <c r="R13" s="44"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -2584,7 +2589,7 @@
       <c r="M14" s="44"/>
       <c r="R14" s="44"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -2615,7 +2620,7 @@
       <c r="M15" s="44"/>
       <c r="R15" s="44"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2646,7 +2651,7 @@
       <c r="M16" s="44"/>
       <c r="R16" s="44"/>
     </row>
-    <row r="17" spans="1:18" s="44" customFormat="1">
+    <row r="17" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
       <c r="C17" s="17"/>
@@ -2656,7 +2661,7 @@
       <c r="G17" s="41"/>
       <c r="H17" s="41"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -2685,7 +2690,7 @@
       <c r="M18" s="44"/>
       <c r="R18" s="44"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -2714,7 +2719,7 @@
       <c r="M19" s="44"/>
       <c r="R19" s="44"/>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -2743,7 +2748,7 @@
       <c r="M20" s="44"/>
       <c r="R20" s="44"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -2772,7 +2777,7 @@
       <c r="M21" s="44"/>
       <c r="R21" s="44"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -2801,7 +2806,7 @@
       <c r="M22" s="44"/>
       <c r="R22" s="44"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -2830,7 +2835,7 @@
       <c r="M23" s="44"/>
       <c r="R23" s="44"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -2861,7 +2866,7 @@
       <c r="M24" s="44"/>
       <c r="R24" s="44"/>
     </row>
-    <row r="25" spans="1:18">
+    <row r="25" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -2892,7 +2897,7 @@
       <c r="M25" s="44"/>
       <c r="R25" s="44"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -2923,7 +2928,7 @@
       <c r="M26" s="44"/>
       <c r="R26" s="44"/>
     </row>
-    <row r="27" spans="1:18" s="44" customFormat="1">
+    <row r="27" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="42"/>
       <c r="B27" s="42"/>
       <c r="C27" s="17"/>
@@ -2933,7 +2938,7 @@
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -2958,7 +2963,7 @@
       <c r="M28" s="44"/>
       <c r="R28" s="44"/>
     </row>
-    <row r="29" spans="1:18" s="44" customFormat="1">
+    <row r="29" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="42"/>
       <c r="B29" s="42"/>
       <c r="C29" s="17"/>
@@ -2968,7 +2973,7 @@
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>35</v>
       </c>
@@ -2997,7 +3002,7 @@
       <c r="M30" s="44"/>
       <c r="R30" s="44"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="47" t="s">
         <v>35</v>
       </c>
@@ -3026,7 +3031,7 @@
       <c r="M31" s="44"/>
       <c r="R31" s="44"/>
     </row>
-    <row r="32" spans="1:18" s="44" customFormat="1">
+    <row r="32" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="42"/>
       <c r="B32" s="42"/>
       <c r="C32" s="17"/>
@@ -3036,7 +3041,7 @@
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
     </row>
-    <row r="33" spans="1:18" s="44" customFormat="1">
+    <row r="33" spans="1:18" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>103</v>
       </c>
@@ -3065,7 +3070,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="44" customFormat="1">
+    <row r="34" spans="1:18" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>103</v>
       </c>
@@ -3089,7 +3094,7 @@
         <v>-70.778433333333339</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="44" customFormat="1">
+    <row r="35" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="42"/>
       <c r="B35" s="42"/>
       <c r="C35" s="17"/>
@@ -3099,7 +3104,7 @@
       <c r="G35" s="41"/>
       <c r="H35" s="41"/>
     </row>
-    <row r="36" spans="1:18">
+    <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="12" t="s">
         <v>36</v>
       </c>
@@ -3128,7 +3133,7 @@
       <c r="M36" s="44"/>
       <c r="R36" s="44"/>
     </row>
-    <row r="37" spans="1:18">
+    <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
         <v>36</v>
       </c>
@@ -3156,7 +3161,7 @@
       <c r="I37" s="1"/>
       <c r="M37" s="44"/>
     </row>
-    <row r="38" spans="1:18" s="44" customFormat="1">
+    <row r="38" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="42"/>
       <c r="B38" s="42"/>
       <c r="C38" s="17"/>
@@ -3166,7 +3171,7 @@
       <c r="G38" s="41"/>
       <c r="H38" s="41"/>
     </row>
-    <row r="39" spans="1:18">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I39" s="12" t="s">
         <v>104</v>
       </c>
@@ -3183,7 +3188,7 @@
       <c r="N39" s="117"/>
       <c r="O39" s="123"/>
     </row>
-    <row r="40" spans="1:18">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
       <c r="I40" s="47" t="s">
         <v>104</v>
       </c>
@@ -3199,7 +3204,7 @@
       <c r="M40" s="44"/>
       <c r="N40" s="118"/>
     </row>
-    <row r="41" spans="1:18" s="44" customFormat="1">
+    <row r="41" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="42"/>
       <c r="B41" s="42"/>
       <c r="C41" s="17"/>
@@ -3209,7 +3214,7 @@
       <c r="G41" s="41"/>
       <c r="H41" s="41"/>
     </row>
-    <row r="42" spans="1:18">
+    <row r="42" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I42" s="15" t="s">
         <v>37</v>
       </c>
@@ -3225,7 +3230,7 @@
       <c r="M42" s="44"/>
       <c r="N42" s="94"/>
     </row>
-    <row r="43" spans="1:18">
+    <row r="43" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I43" s="48" t="s">
         <v>37</v>
       </c>
@@ -3241,7 +3246,7 @@
       <c r="M43" s="44"/>
       <c r="N43" s="94"/>
     </row>
-    <row r="44" spans="1:18">
+    <row r="44" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I44" s="48" t="s">
         <v>37</v>
       </c>
@@ -3257,7 +3262,7 @@
       <c r="M44" s="44"/>
       <c r="N44" s="94"/>
     </row>
-    <row r="45" spans="1:18">
+    <row r="45" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I45" s="48" t="s">
         <v>37</v>
       </c>
@@ -3273,7 +3278,7 @@
       <c r="M45" s="44"/>
       <c r="N45" s="94"/>
     </row>
-    <row r="46" spans="1:18">
+    <row r="46" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I46" s="48" t="s">
         <v>37</v>
       </c>
@@ -3289,7 +3294,7 @@
       <c r="M46" s="44"/>
       <c r="N46" s="95"/>
     </row>
-    <row r="47" spans="1:18">
+    <row r="47" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I47" s="48" t="s">
         <v>37</v>
       </c>
@@ -3305,7 +3310,7 @@
       <c r="M47" s="44"/>
       <c r="N47" s="95"/>
     </row>
-    <row r="48" spans="1:18" s="44" customFormat="1">
+    <row r="48" spans="1:18" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I48" s="48" t="s">
         <v>37</v>
       </c>
@@ -3320,7 +3325,7 @@
       </c>
       <c r="N48" s="67"/>
     </row>
-    <row r="49" spans="1:15">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="18"/>
       <c r="B49" s="42"/>
       <c r="C49" s="17"/>
@@ -3331,7 +3336,7 @@
       <c r="I49" s="1"/>
       <c r="M49" s="44"/>
     </row>
-    <row r="50" spans="1:15">
+    <row r="50" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I50" s="15" t="s">
         <v>38</v>
       </c>
@@ -3348,7 +3353,7 @@
       <c r="N50" s="94"/>
       <c r="O50" s="123"/>
     </row>
-    <row r="51" spans="1:15">
+    <row r="51" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I51" s="48" t="s">
         <v>38</v>
       </c>
@@ -3364,7 +3369,7 @@
       <c r="M51" s="44"/>
       <c r="N51" s="94"/>
     </row>
-    <row r="52" spans="1:15">
+    <row r="52" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I52" s="48" t="s">
         <v>38</v>
       </c>
@@ -3380,7 +3385,7 @@
       <c r="M52" s="44"/>
       <c r="N52" s="94"/>
     </row>
-    <row r="53" spans="1:15">
+    <row r="53" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I53" s="48" t="s">
         <v>38</v>
       </c>
@@ -3396,7 +3401,7 @@
       <c r="M53" s="44"/>
       <c r="N53" s="94"/>
     </row>
-    <row r="54" spans="1:15">
+    <row r="54" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I54" s="48" t="s">
         <v>38</v>
       </c>
@@ -3412,7 +3417,7 @@
       <c r="M54" s="44"/>
       <c r="N54" s="95"/>
     </row>
-    <row r="55" spans="1:15">
+    <row r="55" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I55" s="48" t="s">
         <v>38</v>
       </c>
@@ -3428,7 +3433,7 @@
       <c r="M55" s="44"/>
       <c r="N55" s="95"/>
     </row>
-    <row r="56" spans="1:15" s="44" customFormat="1">
+    <row r="56" spans="1:15" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I56" s="48" t="s">
         <v>38</v>
       </c>
@@ -3443,7 +3448,7 @@
       </c>
       <c r="N56" s="67"/>
     </row>
-    <row r="57" spans="1:15">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="18"/>
       <c r="B57" s="42"/>
       <c r="C57" s="17"/>
@@ -3454,7 +3459,7 @@
       <c r="I57" s="1"/>
       <c r="M57" s="44"/>
     </row>
-    <row r="58" spans="1:15">
+    <row r="58" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
         <v>39</v>
       </c>
@@ -3482,7 +3487,7 @@
       <c r="I58" s="1"/>
       <c r="M58" s="44"/>
     </row>
-    <row r="59" spans="1:15">
+    <row r="59" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="49" t="s">
         <v>39</v>
       </c>
@@ -3510,7 +3515,7 @@
       <c r="I59" s="1"/>
       <c r="M59" s="44"/>
     </row>
-    <row r="60" spans="1:15">
+    <row r="60" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="49" t="s">
         <v>39</v>
       </c>
@@ -3538,7 +3543,7 @@
       <c r="I60" s="1"/>
       <c r="M60" s="44"/>
     </row>
-    <row r="61" spans="1:15">
+    <row r="61" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="49" t="s">
         <v>39</v>
       </c>
@@ -3566,7 +3571,7 @@
       <c r="I61" s="1"/>
       <c r="M61" s="44"/>
     </row>
-    <row r="62" spans="1:15">
+    <row r="62" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="49" t="s">
         <v>39</v>
       </c>
@@ -3594,7 +3599,7 @@
       <c r="I62" s="1"/>
       <c r="M62" s="44"/>
     </row>
-    <row r="63" spans="1:15">
+    <row r="63" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="49" t="s">
         <v>39</v>
       </c>
@@ -3622,7 +3627,7 @@
       <c r="I63" s="1"/>
       <c r="M63" s="44"/>
     </row>
-    <row r="64" spans="1:15">
+    <row r="64" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="49" t="s">
         <v>39</v>
       </c>
@@ -3650,7 +3655,7 @@
       <c r="I64" s="1"/>
       <c r="M64" s="44"/>
     </row>
-    <row r="65" spans="1:15" s="21" customFormat="1">
+    <row r="65" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="49" t="s">
         <v>39</v>
       </c>
@@ -3677,7 +3682,7 @@
       </c>
       <c r="M65" s="44"/>
     </row>
-    <row r="66" spans="1:15">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="18"/>
       <c r="B66" s="42"/>
       <c r="C66" s="17"/>
@@ -3688,7 +3693,7 @@
       <c r="I66" s="1"/>
       <c r="M66" s="44"/>
     </row>
-    <row r="67" spans="1:15">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I67" s="19" t="s">
         <v>40</v>
       </c>
@@ -3705,7 +3710,7 @@
       <c r="N67" s="94"/>
       <c r="O67" s="123"/>
     </row>
-    <row r="68" spans="1:15">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I68" s="49" t="s">
         <v>40</v>
       </c>
@@ -3721,7 +3726,7 @@
       <c r="M68" s="44"/>
       <c r="N68" s="94"/>
     </row>
-    <row r="69" spans="1:15">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I69" s="49" t="s">
         <v>40</v>
       </c>
@@ -3737,7 +3742,7 @@
       <c r="M69" s="44"/>
       <c r="N69" s="94"/>
     </row>
-    <row r="70" spans="1:15">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I70" s="49" t="s">
         <v>40</v>
       </c>
@@ -3753,7 +3758,7 @@
       <c r="M70" s="44"/>
       <c r="N70" s="94"/>
     </row>
-    <row r="71" spans="1:15">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I71" s="49" t="s">
         <v>40</v>
       </c>
@@ -3769,7 +3774,7 @@
       <c r="M71" s="44"/>
       <c r="N71" s="94"/>
     </row>
-    <row r="72" spans="1:15">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I72" s="49" t="s">
         <v>40</v>
       </c>
@@ -3785,7 +3790,7 @@
       <c r="M72" s="44"/>
       <c r="N72" s="94"/>
     </row>
-    <row r="73" spans="1:15">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I73" s="49" t="s">
         <v>40</v>
       </c>
@@ -3801,7 +3806,7 @@
       <c r="M73" s="44"/>
       <c r="N73" s="94"/>
     </row>
-    <row r="74" spans="1:15">
+    <row r="74" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I74" s="49" t="s">
         <v>40</v>
       </c>
@@ -3817,7 +3822,7 @@
       <c r="M74" s="44"/>
       <c r="N74" s="94"/>
     </row>
-    <row r="75" spans="1:15">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="18"/>
       <c r="B75" s="42"/>
       <c r="C75" s="17"/>
@@ -3828,7 +3833,7 @@
       <c r="I75" s="1"/>
       <c r="M75" s="44"/>
     </row>
-    <row r="76" spans="1:15">
+    <row r="76" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="23" t="s">
         <v>43</v>
       </c>
@@ -3856,7 +3861,7 @@
       <c r="I76" s="1"/>
       <c r="M76" s="44"/>
     </row>
-    <row r="77" spans="1:15">
+    <row r="77" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="50" t="s">
         <v>43</v>
       </c>
@@ -3884,7 +3889,7 @@
       <c r="I77" s="1"/>
       <c r="M77" s="44"/>
     </row>
-    <row r="78" spans="1:15">
+    <row r="78" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="50" t="s">
         <v>43</v>
       </c>
@@ -3912,7 +3917,7 @@
       <c r="I78" s="1"/>
       <c r="M78" s="44"/>
     </row>
-    <row r="79" spans="1:15">
+    <row r="79" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="50" t="s">
         <v>43</v>
       </c>
@@ -3940,7 +3945,7 @@
       <c r="I79" s="1"/>
       <c r="M79" s="44"/>
     </row>
-    <row r="80" spans="1:15">
+    <row r="80" spans="1:15" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="50" t="s">
         <v>43</v>
       </c>
@@ -3968,7 +3973,7 @@
       <c r="I80" s="1"/>
       <c r="M80" s="44"/>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="50" t="s">
         <v>43</v>
       </c>
@@ -3996,7 +4001,7 @@
       <c r="I81" s="1"/>
       <c r="M81" s="44"/>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="50" t="s">
         <v>43</v>
       </c>
@@ -4019,14 +4024,14 @@
         <v>98</v>
       </c>
       <c r="H82" s="68">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>102</v>
       </c>
       <c r="M82" s="44"/>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="50" t="s">
         <v>43</v>
       </c>
@@ -4056,7 +4061,7 @@
       </c>
       <c r="M83" s="44"/>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="50" t="s">
         <v>43</v>
       </c>
@@ -4086,7 +4091,7 @@
       </c>
       <c r="M84" s="44"/>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="50" t="s">
         <v>43</v>
       </c>
@@ -4116,7 +4121,7 @@
       </c>
       <c r="M85" s="44"/>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" s="18"/>
       <c r="B86" s="42"/>
       <c r="C86" s="17"/>
@@ -4127,7 +4132,7 @@
       <c r="I86" s="1"/>
       <c r="M86" s="44"/>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="19" t="s">
         <v>44</v>
       </c>
@@ -4155,7 +4160,7 @@
       <c r="I87" s="1"/>
       <c r="M87" s="44"/>
     </row>
-    <row r="88" spans="1:13" s="40" customFormat="1">
+    <row r="88" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="49" t="s">
         <v>44</v>
       </c>
@@ -4182,7 +4187,7 @@
       </c>
       <c r="M88" s="44"/>
     </row>
-    <row r="89" spans="1:13" s="40" customFormat="1">
+    <row r="89" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="49" t="s">
         <v>44</v>
       </c>
@@ -4209,7 +4214,7 @@
       </c>
       <c r="M89" s="44"/>
     </row>
-    <row r="90" spans="1:13" s="40" customFormat="1">
+    <row r="90" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="49" t="s">
         <v>44</v>
       </c>
@@ -4236,7 +4241,7 @@
       </c>
       <c r="M90" s="44"/>
     </row>
-    <row r="91" spans="1:13" s="40" customFormat="1">
+    <row r="91" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="49" t="s">
         <v>44</v>
       </c>
@@ -4263,7 +4268,7 @@
       </c>
       <c r="M91" s="44"/>
     </row>
-    <row r="92" spans="1:13" s="40" customFormat="1">
+    <row r="92" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="49" t="s">
         <v>44</v>
       </c>
@@ -4290,7 +4295,7 @@
       </c>
       <c r="M92" s="44"/>
     </row>
-    <row r="93" spans="1:13" s="40" customFormat="1">
+    <row r="93" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="49" t="s">
         <v>44</v>
       </c>
@@ -4317,7 +4322,7 @@
       </c>
       <c r="M93" s="44"/>
     </row>
-    <row r="94" spans="1:13" s="40" customFormat="1">
+    <row r="94" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="49" t="s">
         <v>44</v>
       </c>
@@ -4344,7 +4349,7 @@
       </c>
       <c r="M94" s="44"/>
     </row>
-    <row r="95" spans="1:13" s="40" customFormat="1">
+    <row r="95" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="49" t="s">
         <v>44</v>
       </c>
@@ -4371,7 +4376,7 @@
       </c>
       <c r="M95" s="44"/>
     </row>
-    <row r="96" spans="1:13" s="40" customFormat="1">
+    <row r="96" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="49" t="s">
         <v>44</v>
       </c>
@@ -4398,7 +4403,7 @@
       </c>
       <c r="M96" s="44"/>
     </row>
-    <row r="97" spans="1:15" s="40" customFormat="1">
+    <row r="97" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="49" t="s">
         <v>44</v>
       </c>
@@ -4425,7 +4430,7 @@
       </c>
       <c r="M97" s="44"/>
     </row>
-    <row r="98" spans="1:15" s="40" customFormat="1">
+    <row r="98" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="49" t="s">
         <v>44</v>
       </c>
@@ -4452,7 +4457,7 @@
       </c>
       <c r="M98" s="44"/>
     </row>
-    <row r="99" spans="1:15" s="40" customFormat="1">
+    <row r="99" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="49" t="s">
         <v>44</v>
       </c>
@@ -4479,7 +4484,7 @@
       </c>
       <c r="M99" s="44"/>
     </row>
-    <row r="100" spans="1:15" s="40" customFormat="1">
+    <row r="100" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="49" t="s">
         <v>44</v>
       </c>
@@ -4506,7 +4511,7 @@
       </c>
       <c r="M100" s="44"/>
     </row>
-    <row r="101" spans="1:15" s="40" customFormat="1">
+    <row r="101" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="49" t="s">
         <v>44</v>
       </c>
@@ -4533,7 +4538,7 @@
       </c>
       <c r="M101" s="44"/>
     </row>
-    <row r="102" spans="1:15" s="40" customFormat="1">
+    <row r="102" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="49" t="s">
         <v>44</v>
       </c>
@@ -4560,7 +4565,7 @@
       </c>
       <c r="M102" s="44"/>
     </row>
-    <row r="103" spans="1:15" s="40" customFormat="1">
+    <row r="103" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="49" t="s">
         <v>44</v>
       </c>
@@ -4587,7 +4592,7 @@
       </c>
       <c r="M103" s="44"/>
     </row>
-    <row r="104" spans="1:15" s="40" customFormat="1">
+    <row r="104" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="49" t="s">
         <v>44</v>
       </c>
@@ -4614,7 +4619,7 @@
       </c>
       <c r="M104" s="44"/>
     </row>
-    <row r="105" spans="1:15" s="40" customFormat="1">
+    <row r="105" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="49" t="s">
         <v>44</v>
       </c>
@@ -4641,7 +4646,7 @@
       </c>
       <c r="M105" s="44"/>
     </row>
-    <row r="106" spans="1:15" s="40" customFormat="1">
+    <row r="106" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="49" t="s">
         <v>44</v>
       </c>
@@ -4668,7 +4673,7 @@
       </c>
       <c r="M106" s="44"/>
     </row>
-    <row r="107" spans="1:15" s="40" customFormat="1">
+    <row r="107" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="49" t="s">
         <v>44</v>
       </c>
@@ -4695,7 +4700,7 @@
       </c>
       <c r="M107" s="44"/>
     </row>
-    <row r="108" spans="1:15" s="40" customFormat="1">
+    <row r="108" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="49" t="s">
         <v>44</v>
       </c>
@@ -4722,7 +4727,7 @@
       </c>
       <c r="M108" s="44"/>
     </row>
-    <row r="109" spans="1:15" s="40" customFormat="1">
+    <row r="109" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="49" t="s">
         <v>44</v>
       </c>
@@ -4749,7 +4754,7 @@
       </c>
       <c r="M109" s="44"/>
     </row>
-    <row r="110" spans="1:15" s="40" customFormat="1">
+    <row r="110" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="49" t="s">
         <v>44</v>
       </c>
@@ -4776,7 +4781,7 @@
       </c>
       <c r="M110" s="44"/>
     </row>
-    <row r="111" spans="1:15" s="44" customFormat="1">
+    <row r="111" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A111" s="43"/>
       <c r="B111" s="43"/>
       <c r="C111" s="17"/>
@@ -4786,7 +4791,7 @@
       <c r="G111" s="41"/>
       <c r="H111" s="39"/>
     </row>
-    <row r="112" spans="1:15">
+    <row r="112" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I112" s="19" t="s">
         <v>45</v>
       </c>
@@ -4803,7 +4808,7 @@
       <c r="N112" s="98"/>
       <c r="O112" s="123"/>
     </row>
-    <row r="113" spans="9:14">
+    <row r="113" spans="9:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I113" s="49" t="s">
         <v>45</v>
       </c>
@@ -4819,7 +4824,7 @@
       <c r="M113" s="44"/>
       <c r="N113" s="99"/>
     </row>
-    <row r="114" spans="9:14" s="44" customFormat="1">
+    <row r="114" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I114" s="49" t="s">
         <v>45</v>
       </c>
@@ -4834,7 +4839,7 @@
       </c>
       <c r="N114" s="96"/>
     </row>
-    <row r="115" spans="9:14" s="44" customFormat="1">
+    <row r="115" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I115" s="49" t="s">
         <v>45</v>
       </c>
@@ -4849,7 +4854,7 @@
       </c>
       <c r="N115" s="96"/>
     </row>
-    <row r="116" spans="9:14" s="44" customFormat="1">
+    <row r="116" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I116" s="49" t="s">
         <v>45</v>
       </c>
@@ -4864,7 +4869,7 @@
       </c>
       <c r="N116" s="96"/>
     </row>
-    <row r="117" spans="9:14" s="44" customFormat="1">
+    <row r="117" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I117" s="49" t="s">
         <v>45</v>
       </c>
@@ -4879,7 +4884,7 @@
       </c>
       <c r="N117" s="96"/>
     </row>
-    <row r="118" spans="9:14" s="44" customFormat="1">
+    <row r="118" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I118" s="49" t="s">
         <v>45</v>
       </c>
@@ -4894,7 +4899,7 @@
       </c>
       <c r="N118" s="100"/>
     </row>
-    <row r="119" spans="9:14" s="44" customFormat="1">
+    <row r="119" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I119" s="49" t="s">
         <v>45</v>
       </c>
@@ -4909,7 +4914,7 @@
       </c>
       <c r="N119" s="96"/>
     </row>
-    <row r="120" spans="9:14" s="44" customFormat="1">
+    <row r="120" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I120" s="49" t="s">
         <v>45</v>
       </c>
@@ -4924,7 +4929,7 @@
       </c>
       <c r="N120" s="97"/>
     </row>
-    <row r="121" spans="9:14" s="44" customFormat="1">
+    <row r="121" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I121" s="49" t="s">
         <v>45</v>
       </c>
@@ -4939,7 +4944,7 @@
       </c>
       <c r="N121" s="97"/>
     </row>
-    <row r="122" spans="9:14" s="44" customFormat="1">
+    <row r="122" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I122" s="49" t="s">
         <v>45</v>
       </c>
@@ -4954,7 +4959,7 @@
       </c>
       <c r="N122" s="97"/>
     </row>
-    <row r="123" spans="9:14" s="44" customFormat="1">
+    <row r="123" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I123" s="49" t="s">
         <v>45</v>
       </c>
@@ -4969,7 +4974,7 @@
       </c>
       <c r="N123" s="97"/>
     </row>
-    <row r="124" spans="9:14" s="44" customFormat="1">
+    <row r="124" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I124" s="49" t="s">
         <v>45</v>
       </c>
@@ -4984,7 +4989,7 @@
       </c>
       <c r="N124" s="97"/>
     </row>
-    <row r="125" spans="9:14" s="44" customFormat="1">
+    <row r="125" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I125" s="49" t="s">
         <v>45</v>
       </c>
@@ -4999,7 +5004,7 @@
       </c>
       <c r="N125" s="97"/>
     </row>
-    <row r="126" spans="9:14" s="44" customFormat="1">
+    <row r="126" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I126" s="49" t="s">
         <v>45</v>
       </c>
@@ -5014,7 +5019,7 @@
       </c>
       <c r="N126" s="97"/>
     </row>
-    <row r="127" spans="9:14" s="44" customFormat="1">
+    <row r="127" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I127" s="49" t="s">
         <v>45</v>
       </c>
@@ -5029,7 +5034,7 @@
       </c>
       <c r="N127" s="97"/>
     </row>
-    <row r="128" spans="9:14" s="44" customFormat="1">
+    <row r="128" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I128" s="49" t="s">
         <v>45</v>
       </c>
@@ -5044,7 +5049,7 @@
       </c>
       <c r="N128" s="97"/>
     </row>
-    <row r="129" spans="1:15" s="44" customFormat="1">
+    <row r="129" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I129" s="49" t="s">
         <v>45</v>
       </c>
@@ -5059,7 +5064,7 @@
       </c>
       <c r="N129" s="97"/>
     </row>
-    <row r="130" spans="1:15" s="44" customFormat="1">
+    <row r="130" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I130" s="49" t="s">
         <v>45</v>
       </c>
@@ -5074,7 +5079,7 @@
       </c>
       <c r="N130" s="97"/>
     </row>
-    <row r="131" spans="1:15" s="44" customFormat="1">
+    <row r="131" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I131" s="49" t="s">
         <v>45</v>
       </c>
@@ -5089,7 +5094,7 @@
       </c>
       <c r="N131" s="97"/>
     </row>
-    <row r="132" spans="1:15" s="44" customFormat="1">
+    <row r="132" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I132" s="49" t="s">
         <v>45</v>
       </c>
@@ -5104,7 +5109,7 @@
       </c>
       <c r="N132" s="96"/>
     </row>
-    <row r="133" spans="1:15" s="44" customFormat="1">
+    <row r="133" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I133" s="49" t="s">
         <v>45</v>
       </c>
@@ -5119,7 +5124,7 @@
       </c>
       <c r="N133" s="97"/>
     </row>
-    <row r="134" spans="1:15" s="44" customFormat="1">
+    <row r="134" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I134" s="49" t="s">
         <v>45</v>
       </c>
@@ -5134,7 +5139,7 @@
       </c>
       <c r="N134" s="97"/>
     </row>
-    <row r="135" spans="1:15" s="44" customFormat="1">
+    <row r="135" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I135" s="49" t="s">
         <v>45</v>
       </c>
@@ -5149,7 +5154,7 @@
       </c>
       <c r="N135" s="97"/>
     </row>
-    <row r="136" spans="1:15">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" s="18"/>
       <c r="B136" s="42"/>
       <c r="C136" s="17"/>
@@ -5160,7 +5165,7 @@
       <c r="I136" s="1"/>
       <c r="M136" s="44"/>
     </row>
-    <row r="137" spans="1:15">
+    <row r="137" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="16" t="s">
         <v>46</v>
       </c>
@@ -5188,7 +5193,7 @@
       <c r="I137" s="1"/>
       <c r="M137" s="44"/>
     </row>
-    <row r="138" spans="1:15">
+    <row r="138" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="51" t="s">
         <v>46</v>
       </c>
@@ -5216,7 +5221,7 @@
       <c r="I138" s="1"/>
       <c r="M138" s="44"/>
     </row>
-    <row r="139" spans="1:15">
+    <row r="139" spans="1:15" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="51" t="s">
         <v>46</v>
       </c>
@@ -5244,7 +5249,7 @@
       <c r="I139" s="1"/>
       <c r="M139" s="44"/>
     </row>
-    <row r="140" spans="1:15" s="44" customFormat="1">
+    <row r="140" spans="1:15" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="85" t="s">
         <v>46</v>
       </c>
@@ -5268,7 +5273,7 @@
       </c>
       <c r="H140" s="102"/>
     </row>
-    <row r="141" spans="1:15">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" s="18"/>
       <c r="B141" s="42"/>
       <c r="C141" s="17"/>
@@ -5279,7 +5284,7 @@
       <c r="I141" s="1"/>
       <c r="M141" s="44"/>
     </row>
-    <row r="142" spans="1:15">
+    <row r="142" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I142" s="16" t="s">
         <v>47</v>
       </c>
@@ -5296,7 +5301,7 @@
       <c r="N142" s="103"/>
       <c r="O142" s="123"/>
     </row>
-    <row r="143" spans="1:15">
+    <row r="143" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I143" s="51" t="s">
         <v>47</v>
       </c>
@@ -5312,7 +5317,7 @@
       <c r="M143" s="44"/>
       <c r="N143" s="103"/>
     </row>
-    <row r="144" spans="1:15">
+    <row r="144" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
       <c r="I144" s="51" t="s">
         <v>47</v>
       </c>
@@ -5328,7 +5333,7 @@
       <c r="M144" s="44"/>
       <c r="N144" s="104"/>
     </row>
-    <row r="145" spans="1:22" s="44" customFormat="1">
+    <row r="145" spans="1:22" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I145" s="85" t="s">
         <v>47</v>
       </c>
@@ -5343,7 +5348,7 @@
       </c>
       <c r="N145" s="105"/>
     </row>
-    <row r="146" spans="1:22">
+    <row r="146" spans="1:22" x14ac:dyDescent="0.2">
       <c r="I146" s="18"/>
       <c r="J146" s="17"/>
       <c r="K146" s="45"/>
@@ -5351,7 +5356,7 @@
       <c r="M146" s="44"/>
       <c r="N146" s="29"/>
     </row>
-    <row r="147" spans="1:22">
+    <row r="147" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="119" t="s">
         <v>136</v>
       </c>
@@ -5381,7 +5386,7 @@
       </c>
       <c r="M147" s="44"/>
     </row>
-    <row r="148" spans="1:22">
+    <row r="148" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="50" t="s">
         <v>136</v>
       </c>
@@ -5411,7 +5416,7 @@
       </c>
       <c r="M148" s="44"/>
     </row>
-    <row r="149" spans="1:22">
+    <row r="149" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="50" t="s">
         <v>136</v>
       </c>
@@ -5439,7 +5444,7 @@
       <c r="I149" s="1"/>
       <c r="M149" s="44"/>
     </row>
-    <row r="150" spans="1:22">
+    <row r="150" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="50" t="s">
         <v>136</v>
       </c>
@@ -5467,7 +5472,7 @@
       <c r="I150" s="1"/>
       <c r="M150" s="44"/>
     </row>
-    <row r="151" spans="1:22">
+    <row r="151" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="50" t="s">
         <v>136</v>
       </c>
@@ -5495,7 +5500,7 @@
       <c r="I151" s="1"/>
       <c r="M151" s="44"/>
     </row>
-    <row r="152" spans="1:22">
+    <row r="152" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="50" t="s">
         <v>136</v>
       </c>
@@ -5523,7 +5528,7 @@
       <c r="I152" s="1"/>
       <c r="M152" s="44"/>
     </row>
-    <row r="153" spans="1:22">
+    <row r="153" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="50" t="s">
         <v>136</v>
       </c>
@@ -5551,7 +5556,7 @@
       <c r="I153" s="1"/>
       <c r="M153" s="44"/>
     </row>
-    <row r="154" spans="1:22">
+    <row r="154" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A154" s="18"/>
       <c r="B154" s="42"/>
       <c r="C154" s="17"/>
@@ -5562,7 +5567,7 @@
       <c r="I154" s="1"/>
       <c r="M154" s="44"/>
     </row>
-    <row r="155" spans="1:22">
+    <row r="155" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A155" s="33" t="s">
         <v>137</v>
       </c>
@@ -5594,7 +5599,7 @@
       <c r="U155" s="40"/>
       <c r="V155" s="40"/>
     </row>
-    <row r="156" spans="1:22">
+    <row r="156" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A156" s="52" t="s">
         <v>137</v>
       </c>
@@ -5626,7 +5631,7 @@
       <c r="U156" s="40"/>
       <c r="V156" s="40"/>
     </row>
-    <row r="157" spans="1:22">
+    <row r="157" spans="1:22" ht="15" x14ac:dyDescent="0.25">
       <c r="A157" s="52" t="s">
         <v>137</v>
       </c>
@@ -5654,7 +5659,7 @@
       <c r="I157" s="1"/>
       <c r="M157" s="44"/>
     </row>
-    <row r="158" spans="1:22">
+    <row r="158" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A158" s="18"/>
       <c r="B158" s="42"/>
       <c r="C158" s="17"/>
@@ -5665,7 +5670,7 @@
       <c r="I158" s="1"/>
       <c r="M158" s="44"/>
     </row>
-    <row r="159" spans="1:22">
+    <row r="159" spans="1:22" x14ac:dyDescent="0.2">
       <c r="I159" s="34" t="s">
         <v>58</v>
       </c>
@@ -5682,7 +5687,7 @@
       <c r="N159" s="107"/>
       <c r="O159" s="123"/>
     </row>
-    <row r="160" spans="1:22">
+    <row r="160" spans="1:22" x14ac:dyDescent="0.2">
       <c r="I160" s="52" t="s">
         <v>58</v>
       </c>
@@ -5698,7 +5703,7 @@
       <c r="M160" s="44"/>
       <c r="N160" s="98"/>
     </row>
-    <row r="161" spans="9:22">
+    <row r="161" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I161" s="52" t="s">
         <v>58</v>
       </c>
@@ -5714,7 +5719,7 @@
       <c r="M161" s="44"/>
       <c r="N161" s="99"/>
     </row>
-    <row r="162" spans="9:22">
+    <row r="162" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I162" s="52" t="s">
         <v>58</v>
       </c>
@@ -5733,7 +5738,7 @@
       <c r="U162" s="44"/>
       <c r="V162" s="44"/>
     </row>
-    <row r="163" spans="9:22">
+    <row r="163" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I163" s="52" t="s">
         <v>58</v>
       </c>
@@ -5749,7 +5754,7 @@
       <c r="M163" s="44"/>
       <c r="N163" s="107"/>
     </row>
-    <row r="164" spans="9:22">
+    <row r="164" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I164" s="52" t="s">
         <v>58</v>
       </c>
@@ -5765,7 +5770,7 @@
       <c r="M164" s="44"/>
       <c r="N164" s="107"/>
     </row>
-    <row r="165" spans="9:22">
+    <row r="165" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I165" s="52" t="s">
         <v>58</v>
       </c>
@@ -5781,7 +5786,7 @@
       <c r="M165" s="44"/>
       <c r="N165" s="107"/>
     </row>
-    <row r="166" spans="9:22">
+    <row r="166" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I166" s="18"/>
       <c r="J166" s="17"/>
       <c r="K166" s="45"/>
@@ -5789,7 +5794,7 @@
       <c r="M166" s="44"/>
       <c r="N166" s="18"/>
     </row>
-    <row r="167" spans="9:22">
+    <row r="167" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I167" s="34" t="s">
         <v>59</v>
       </c>
@@ -5806,7 +5811,7 @@
       <c r="N167" s="108"/>
       <c r="O167" s="123"/>
     </row>
-    <row r="168" spans="9:22">
+    <row r="168" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I168" s="52" t="s">
         <v>59</v>
       </c>
@@ -5822,7 +5827,7 @@
       <c r="M168" s="44"/>
       <c r="N168" s="108"/>
     </row>
-    <row r="169" spans="9:22">
+    <row r="169" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I169" s="52" t="s">
         <v>59</v>
       </c>
@@ -5838,7 +5843,7 @@
       <c r="M169" s="44"/>
       <c r="N169" s="108"/>
     </row>
-    <row r="170" spans="9:22">
+    <row r="170" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I170" s="52" t="s">
         <v>59</v>
       </c>
@@ -5854,7 +5859,7 @@
       <c r="M170" s="44"/>
       <c r="N170" s="108"/>
     </row>
-    <row r="171" spans="9:22">
+    <row r="171" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I171" s="52" t="s">
         <v>59</v>
       </c>
@@ -5870,7 +5875,7 @@
       <c r="M171" s="44"/>
       <c r="N171" s="108"/>
     </row>
-    <row r="172" spans="9:22">
+    <row r="172" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I172" s="52" t="s">
         <v>59</v>
       </c>
@@ -5886,7 +5891,7 @@
       <c r="M172" s="44"/>
       <c r="N172" s="71"/>
     </row>
-    <row r="173" spans="9:22">
+    <row r="173" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I173" s="52" t="s">
         <v>59</v>
       </c>
@@ -5902,7 +5907,7 @@
       <c r="M173" s="44"/>
       <c r="N173" s="108"/>
     </row>
-    <row r="174" spans="9:22">
+    <row r="174" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I174" s="52" t="s">
         <v>59</v>
       </c>
@@ -5918,7 +5923,7 @@
       <c r="M174" s="44"/>
       <c r="N174" s="71"/>
     </row>
-    <row r="175" spans="9:22">
+    <row r="175" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I175" s="52" t="s">
         <v>59</v>
       </c>
@@ -5934,7 +5939,7 @@
       <c r="M175" s="44"/>
       <c r="N175" s="108"/>
     </row>
-    <row r="176" spans="9:22">
+    <row r="176" spans="9:22" x14ac:dyDescent="0.2">
       <c r="I176" s="52" t="s">
         <v>59</v>
       </c>
@@ -5950,7 +5955,7 @@
       <c r="M176" s="44"/>
       <c r="N176" s="108"/>
     </row>
-    <row r="177" spans="9:15">
+    <row r="177" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I177" s="52" t="s">
         <v>59</v>
       </c>
@@ -5966,7 +5971,7 @@
       <c r="M177" s="44"/>
       <c r="N177" s="108"/>
     </row>
-    <row r="178" spans="9:15">
+    <row r="178" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I178" s="52" t="s">
         <v>59</v>
       </c>
@@ -5982,7 +5987,7 @@
       <c r="M178" s="44"/>
       <c r="N178" s="108"/>
     </row>
-    <row r="179" spans="9:15">
+    <row r="179" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I179" s="52" t="s">
         <v>59</v>
       </c>
@@ -5998,7 +6003,7 @@
       <c r="M179" s="44"/>
       <c r="N179" s="108"/>
     </row>
-    <row r="180" spans="9:15">
+    <row r="180" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I180" s="52" t="s">
         <v>59</v>
       </c>
@@ -6014,7 +6019,7 @@
       <c r="M180" s="44"/>
       <c r="N180" s="108"/>
     </row>
-    <row r="181" spans="9:15">
+    <row r="181" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I181" s="52" t="s">
         <v>59</v>
       </c>
@@ -6030,7 +6035,7 @@
       <c r="M181" s="44"/>
       <c r="N181" s="108"/>
     </row>
-    <row r="182" spans="9:15">
+    <row r="182" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I182" s="52" t="s">
         <v>59</v>
       </c>
@@ -6046,7 +6051,7 @@
       <c r="M182" s="44"/>
       <c r="N182" s="109"/>
     </row>
-    <row r="183" spans="9:15" s="44" customFormat="1">
+    <row r="183" spans="9:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I183" s="52" t="s">
         <v>59</v>
       </c>
@@ -6061,7 +6066,7 @@
       </c>
       <c r="N183" s="110"/>
     </row>
-    <row r="184" spans="9:15" s="44" customFormat="1">
+    <row r="184" spans="9:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I184" s="52" t="s">
         <v>59</v>
       </c>
@@ -6076,7 +6081,7 @@
       </c>
       <c r="N184" s="110"/>
     </row>
-    <row r="185" spans="9:15">
+    <row r="185" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I185" s="18"/>
       <c r="J185" s="17"/>
       <c r="K185" s="45"/>
@@ -6084,7 +6089,7 @@
       <c r="M185" s="44"/>
       <c r="N185" s="18"/>
     </row>
-    <row r="186" spans="9:15">
+    <row r="186" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I186" s="34" t="s">
         <v>60</v>
       </c>
@@ -6101,7 +6106,7 @@
       <c r="N186" s="111"/>
       <c r="O186" s="123"/>
     </row>
-    <row r="187" spans="9:15">
+    <row r="187" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I187" s="52" t="s">
         <v>60</v>
       </c>
@@ -6117,7 +6122,7 @@
       <c r="M187" s="44"/>
       <c r="N187" s="111"/>
     </row>
-    <row r="188" spans="9:15">
+    <row r="188" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I188" s="52" t="s">
         <v>60</v>
       </c>
@@ -6133,7 +6138,7 @@
       <c r="M188" s="44"/>
       <c r="N188" s="111"/>
     </row>
-    <row r="189" spans="9:15">
+    <row r="189" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I189" s="52" t="s">
         <v>60</v>
       </c>
@@ -6149,7 +6154,7 @@
       <c r="M189" s="44"/>
       <c r="N189" s="111"/>
     </row>
-    <row r="190" spans="9:15">
+    <row r="190" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I190" s="52" t="s">
         <v>60</v>
       </c>
@@ -6165,7 +6170,7 @@
       <c r="M190" s="44"/>
       <c r="N190" s="94"/>
     </row>
-    <row r="191" spans="9:15">
+    <row r="191" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I191" s="52" t="s">
         <v>60</v>
       </c>
@@ -6181,7 +6186,7 @@
       <c r="M191" s="44"/>
       <c r="N191" s="94"/>
     </row>
-    <row r="192" spans="9:15">
+    <row r="192" spans="9:15" x14ac:dyDescent="0.2">
       <c r="I192" s="52" t="s">
         <v>60</v>
       </c>
@@ -6197,7 +6202,7 @@
       <c r="M192" s="44"/>
       <c r="N192" s="94"/>
     </row>
-    <row r="193" spans="1:17">
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I193" s="52" t="s">
         <v>60</v>
       </c>
@@ -6213,7 +6218,7 @@
       <c r="M193" s="44"/>
       <c r="N193" s="94"/>
     </row>
-    <row r="194" spans="1:17">
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A194" s="23"/>
       <c r="B194" s="23"/>
       <c r="C194" s="46"/>
@@ -6222,7 +6227,7 @@
       <c r="I194" s="1"/>
       <c r="M194" s="44"/>
     </row>
-    <row r="195" spans="1:17" s="44" customFormat="1">
+    <row r="195" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="I195" s="79" t="s">
         <v>110</v>
       </c>
@@ -6238,7 +6243,7 @@
       <c r="N195" s="76"/>
       <c r="O195" s="123"/>
     </row>
-    <row r="196" spans="1:17" s="44" customFormat="1">
+    <row r="196" spans="1:17" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A196" s="82"/>
       <c r="B196" s="82"/>
       <c r="C196" s="83"/>
@@ -6252,7 +6257,7 @@
       <c r="N196" s="73"/>
       <c r="O196" s="73"/>
     </row>
-    <row r="197" spans="1:17">
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I197" s="78" t="s">
         <v>109</v>
       </c>
@@ -6271,7 +6276,7 @@
       <c r="P197" s="44"/>
       <c r="Q197" s="44"/>
     </row>
-    <row r="198" spans="1:17" s="44" customFormat="1">
+    <row r="198" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A198" s="23"/>
       <c r="B198" s="23"/>
       <c r="C198" s="17"/>
@@ -6281,7 +6286,7 @@
       <c r="H198" s="45"/>
       <c r="I198" s="72"/>
     </row>
-    <row r="199" spans="1:17">
+    <row r="199" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A199" s="19" t="s">
         <v>85</v>
       </c>
@@ -6305,7 +6310,7 @@
       <c r="I199" s="1"/>
       <c r="M199" s="44"/>
     </row>
-    <row r="200" spans="1:17">
+    <row r="200" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="I200" s="18" t="s">
         <v>83</v>
       </c>
@@ -6321,7 +6326,7 @@
       <c r="M200" s="44"/>
       <c r="N200" s="35"/>
     </row>
-    <row r="201" spans="1:17">
+    <row r="201" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="I201" s="18" t="s">
         <v>84</v>
       </c>
@@ -6338,7 +6343,7 @@
       <c r="N201" s="35"/>
       <c r="O201" s="123"/>
     </row>
-    <row r="202" spans="1:17">
+    <row r="202" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A202" s="18"/>
       <c r="B202" s="42"/>
       <c r="C202" s="17"/>
@@ -6349,7 +6354,7 @@
       <c r="I202" s="1"/>
       <c r="M202" s="44"/>
     </row>
-    <row r="203" spans="1:17">
+    <row r="203" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A203" s="19" t="s">
         <v>91</v>
       </c>
@@ -6374,7 +6379,7 @@
       <c r="J203" s="44"/>
       <c r="M203" s="44"/>
     </row>
-    <row r="204" spans="1:17">
+    <row r="204" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A204" s="18" t="s">
         <v>86</v>
       </c>
@@ -6399,7 +6404,7 @@
       <c r="J204" s="44"/>
       <c r="M204" s="44"/>
     </row>
-    <row r="205" spans="1:17">
+    <row r="205" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A205" s="18" t="s">
         <v>87</v>
       </c>
@@ -6424,7 +6429,7 @@
       <c r="J205" s="44"/>
       <c r="M205" s="44"/>
     </row>
-    <row r="206" spans="1:17">
+    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I206" s="18" t="s">
         <v>88</v>
       </c>
@@ -6441,7 +6446,7 @@
       <c r="N206" s="44"/>
       <c r="O206" s="73"/>
     </row>
-    <row r="207" spans="1:17">
+    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I207" s="18" t="s">
         <v>89</v>
       </c>
@@ -6458,7 +6463,7 @@
       <c r="N207" s="44"/>
       <c r="O207" s="123"/>
     </row>
-    <row r="208" spans="1:17">
+    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I208" s="18" t="s">
         <v>90</v>
       </c>
@@ -6475,633 +6480,633 @@
       <c r="N208" s="44"/>
       <c r="O208" s="123"/>
     </row>
-    <row r="209" spans="9:13">
+    <row r="209" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I209" s="1"/>
       <c r="M209" s="44"/>
     </row>
-    <row r="210" spans="9:13">
+    <row r="210" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I210" s="1"/>
       <c r="M210" s="44"/>
     </row>
-    <row r="211" spans="9:13">
+    <row r="211" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I211" s="1"/>
       <c r="M211" s="44"/>
     </row>
-    <row r="212" spans="9:13">
+    <row r="212" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I212" s="1"/>
       <c r="M212" s="44"/>
     </row>
-    <row r="213" spans="9:13">
+    <row r="213" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I213" s="1"/>
       <c r="M213" s="44"/>
     </row>
-    <row r="214" spans="9:13">
+    <row r="214" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I214" s="1"/>
       <c r="M214" s="44"/>
     </row>
-    <row r="215" spans="9:13">
+    <row r="215" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I215" s="1"/>
       <c r="M215" s="44"/>
     </row>
-    <row r="216" spans="9:13">
+    <row r="216" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I216" s="1"/>
       <c r="M216" s="44"/>
     </row>
-    <row r="217" spans="9:13">
+    <row r="217" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I217" s="1"/>
       <c r="M217" s="44"/>
     </row>
-    <row r="218" spans="9:13">
+    <row r="218" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I218" s="1"/>
       <c r="M218" s="44"/>
     </row>
-    <row r="219" spans="9:13">
+    <row r="219" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I219" s="1"/>
       <c r="M219" s="44"/>
     </row>
-    <row r="220" spans="9:13">
+    <row r="220" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I220" s="1"/>
       <c r="M220" s="44"/>
     </row>
-    <row r="221" spans="9:13">
+    <row r="221" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I221" s="1"/>
       <c r="M221" s="44"/>
     </row>
-    <row r="222" spans="9:13">
+    <row r="222" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I222" s="1"/>
       <c r="M222" s="44"/>
     </row>
-    <row r="223" spans="9:13">
+    <row r="223" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I223" s="1"/>
       <c r="M223" s="44"/>
     </row>
-    <row r="224" spans="9:13">
+    <row r="224" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I224" s="1"/>
       <c r="M224" s="44"/>
     </row>
-    <row r="225" spans="9:13">
+    <row r="225" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I225" s="1"/>
       <c r="M225" s="44"/>
     </row>
-    <row r="226" spans="9:13">
+    <row r="226" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I226" s="1"/>
       <c r="M226" s="44"/>
     </row>
-    <row r="227" spans="9:13">
+    <row r="227" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I227" s="1"/>
       <c r="M227" s="44"/>
     </row>
-    <row r="228" spans="9:13">
+    <row r="228" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I228" s="1"/>
       <c r="M228" s="44"/>
     </row>
-    <row r="229" spans="9:13">
+    <row r="229" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I229" s="1"/>
       <c r="M229" s="44"/>
     </row>
-    <row r="230" spans="9:13">
+    <row r="230" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I230" s="1"/>
       <c r="M230" s="44"/>
     </row>
-    <row r="231" spans="9:13">
+    <row r="231" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I231" s="1"/>
       <c r="M231" s="44"/>
     </row>
-    <row r="232" spans="9:13">
+    <row r="232" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I232" s="1"/>
       <c r="M232" s="44"/>
     </row>
-    <row r="233" spans="9:13">
+    <row r="233" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I233" s="1"/>
       <c r="M233" s="44"/>
     </row>
-    <row r="234" spans="9:13">
+    <row r="234" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I234" s="1"/>
       <c r="M234" s="44"/>
     </row>
-    <row r="235" spans="9:13">
+    <row r="235" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I235" s="1"/>
       <c r="M235" s="44"/>
     </row>
-    <row r="236" spans="9:13">
+    <row r="236" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I236" s="1"/>
       <c r="M236" s="44"/>
     </row>
-    <row r="237" spans="9:13">
+    <row r="237" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I237" s="1"/>
       <c r="M237" s="44"/>
     </row>
-    <row r="238" spans="9:13">
+    <row r="238" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I238" s="1"/>
       <c r="M238" s="44"/>
     </row>
-    <row r="239" spans="9:13">
+    <row r="239" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I239" s="1"/>
       <c r="M239" s="44"/>
     </row>
-    <row r="240" spans="9:13">
+    <row r="240" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I240" s="1"/>
       <c r="M240" s="44"/>
     </row>
-    <row r="241" spans="9:13">
+    <row r="241" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I241" s="1"/>
       <c r="M241" s="44"/>
     </row>
-    <row r="242" spans="9:13">
+    <row r="242" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I242" s="1"/>
       <c r="M242" s="44"/>
     </row>
-    <row r="243" spans="9:13">
+    <row r="243" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I243" s="1"/>
       <c r="M243" s="44"/>
     </row>
-    <row r="244" spans="9:13">
+    <row r="244" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I244" s="1"/>
       <c r="M244" s="44"/>
     </row>
-    <row r="245" spans="9:13">
+    <row r="245" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I245" s="1"/>
       <c r="M245" s="44"/>
     </row>
-    <row r="246" spans="9:13">
+    <row r="246" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I246" s="1"/>
       <c r="M246" s="44"/>
     </row>
-    <row r="247" spans="9:13">
+    <row r="247" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I247" s="1"/>
       <c r="M247" s="44"/>
     </row>
-    <row r="248" spans="9:13">
+    <row r="248" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I248" s="1"/>
       <c r="M248" s="44"/>
     </row>
-    <row r="249" spans="9:13">
+    <row r="249" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I249" s="1"/>
       <c r="M249" s="44"/>
     </row>
-    <row r="250" spans="9:13">
+    <row r="250" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I250" s="1"/>
       <c r="M250" s="44"/>
     </row>
-    <row r="251" spans="9:13">
+    <row r="251" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I251" s="1"/>
       <c r="M251" s="44"/>
     </row>
-    <row r="252" spans="9:13">
+    <row r="252" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I252" s="1"/>
       <c r="M252" s="44"/>
     </row>
-    <row r="253" spans="9:13">
+    <row r="253" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I253" s="1"/>
       <c r="M253" s="44"/>
     </row>
-    <row r="254" spans="9:13">
+    <row r="254" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I254" s="1"/>
       <c r="M254" s="44"/>
     </row>
-    <row r="255" spans="9:13">
+    <row r="255" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I255" s="1"/>
       <c r="M255" s="44"/>
     </row>
-    <row r="256" spans="9:13">
+    <row r="256" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I256" s="1"/>
       <c r="M256" s="44"/>
     </row>
-    <row r="257" spans="9:13">
+    <row r="257" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I257" s="1"/>
       <c r="M257" s="44"/>
     </row>
-    <row r="258" spans="9:13">
+    <row r="258" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I258" s="1"/>
       <c r="M258" s="44"/>
     </row>
-    <row r="259" spans="9:13">
+    <row r="259" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I259" s="1"/>
       <c r="M259" s="44"/>
     </row>
-    <row r="260" spans="9:13">
+    <row r="260" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I260" s="1"/>
       <c r="M260" s="44"/>
     </row>
-    <row r="261" spans="9:13">
+    <row r="261" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I261" s="1"/>
       <c r="M261" s="44"/>
     </row>
-    <row r="262" spans="9:13">
+    <row r="262" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I262" s="1"/>
       <c r="M262" s="44"/>
     </row>
-    <row r="263" spans="9:13">
+    <row r="263" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I263" s="1"/>
       <c r="M263" s="44"/>
     </row>
-    <row r="264" spans="9:13">
+    <row r="264" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I264" s="1"/>
       <c r="M264" s="44"/>
     </row>
-    <row r="265" spans="9:13">
+    <row r="265" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I265" s="1"/>
       <c r="M265" s="44"/>
     </row>
-    <row r="266" spans="9:13">
+    <row r="266" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I266" s="1"/>
       <c r="M266" s="44"/>
     </row>
-    <row r="267" spans="9:13">
+    <row r="267" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I267" s="1"/>
       <c r="M267" s="44"/>
     </row>
-    <row r="268" spans="9:13">
+    <row r="268" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I268" s="1"/>
       <c r="M268" s="44"/>
     </row>
-    <row r="269" spans="9:13">
+    <row r="269" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I269" s="1"/>
       <c r="M269" s="44"/>
     </row>
-    <row r="270" spans="9:13">
+    <row r="270" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I270" s="1"/>
       <c r="M270" s="44"/>
     </row>
-    <row r="271" spans="9:13">
+    <row r="271" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I271" s="1"/>
       <c r="M271" s="44"/>
     </row>
-    <row r="272" spans="9:13">
+    <row r="272" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I272" s="1"/>
       <c r="M272" s="44"/>
     </row>
-    <row r="273" spans="9:13">
+    <row r="273" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I273" s="1"/>
       <c r="M273" s="44"/>
     </row>
-    <row r="274" spans="9:13">
+    <row r="274" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I274" s="1"/>
       <c r="M274" s="44"/>
     </row>
-    <row r="275" spans="9:13">
+    <row r="275" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I275" s="1"/>
       <c r="M275" s="44"/>
     </row>
-    <row r="276" spans="9:13">
+    <row r="276" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I276" s="1"/>
       <c r="M276" s="44"/>
     </row>
-    <row r="277" spans="9:13">
+    <row r="277" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I277" s="1"/>
       <c r="M277" s="44"/>
     </row>
-    <row r="278" spans="9:13">
+    <row r="278" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I278" s="1"/>
       <c r="M278" s="44"/>
     </row>
-    <row r="279" spans="9:13">
+    <row r="279" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I279" s="1"/>
       <c r="M279" s="44"/>
     </row>
-    <row r="280" spans="9:13">
+    <row r="280" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I280" s="1"/>
       <c r="M280" s="44"/>
     </row>
-    <row r="281" spans="9:13">
+    <row r="281" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I281" s="1"/>
       <c r="M281" s="44"/>
     </row>
-    <row r="282" spans="9:13">
+    <row r="282" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I282" s="1"/>
       <c r="M282" s="44"/>
     </row>
-    <row r="283" spans="9:13">
+    <row r="283" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I283" s="1"/>
       <c r="M283" s="44"/>
     </row>
-    <row r="284" spans="9:13">
+    <row r="284" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I284" s="1"/>
       <c r="M284" s="44"/>
     </row>
-    <row r="285" spans="9:13">
+    <row r="285" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I285" s="1"/>
       <c r="M285" s="44"/>
     </row>
-    <row r="286" spans="9:13">
+    <row r="286" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I286" s="1"/>
       <c r="M286" s="44"/>
     </row>
-    <row r="287" spans="9:13">
+    <row r="287" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I287" s="1"/>
       <c r="M287" s="44"/>
     </row>
-    <row r="288" spans="9:13">
+    <row r="288" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I288" s="1"/>
       <c r="M288" s="44"/>
     </row>
-    <row r="289" spans="9:13">
+    <row r="289" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I289" s="1"/>
       <c r="M289" s="44"/>
     </row>
-    <row r="290" spans="9:13">
+    <row r="290" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I290" s="1"/>
       <c r="M290" s="44"/>
     </row>
-    <row r="291" spans="9:13">
+    <row r="291" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I291" s="1"/>
       <c r="M291" s="44"/>
     </row>
-    <row r="292" spans="9:13">
+    <row r="292" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I292" s="1"/>
       <c r="M292" s="44"/>
     </row>
-    <row r="293" spans="9:13">
+    <row r="293" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I293" s="1"/>
       <c r="M293" s="44"/>
     </row>
-    <row r="294" spans="9:13">
+    <row r="294" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I294" s="1"/>
       <c r="M294" s="44"/>
     </row>
-    <row r="295" spans="9:13">
+    <row r="295" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I295" s="1"/>
       <c r="M295" s="44"/>
     </row>
-    <row r="296" spans="9:13">
+    <row r="296" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I296" s="1"/>
       <c r="M296" s="44"/>
     </row>
-    <row r="297" spans="9:13">
+    <row r="297" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I297" s="1"/>
       <c r="M297" s="44"/>
     </row>
-    <row r="298" spans="9:13">
+    <row r="298" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I298" s="1"/>
       <c r="M298" s="44"/>
     </row>
-    <row r="299" spans="9:13">
+    <row r="299" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I299" s="1"/>
       <c r="M299" s="44"/>
     </row>
-    <row r="300" spans="9:13">
+    <row r="300" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I300" s="1"/>
       <c r="M300" s="44"/>
     </row>
-    <row r="301" spans="9:13">
+    <row r="301" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I301" s="1"/>
       <c r="M301" s="44"/>
     </row>
-    <row r="302" spans="9:13">
+    <row r="302" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I302" s="1"/>
       <c r="M302" s="44"/>
     </row>
-    <row r="303" spans="9:13">
+    <row r="303" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I303" s="1"/>
       <c r="M303" s="44"/>
     </row>
-    <row r="304" spans="9:13">
+    <row r="304" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I304" s="1"/>
       <c r="M304" s="44"/>
     </row>
-    <row r="305" spans="9:13">
+    <row r="305" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I305" s="1"/>
       <c r="M305" s="44"/>
     </row>
-    <row r="306" spans="9:13">
+    <row r="306" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I306" s="1"/>
       <c r="M306" s="44"/>
     </row>
-    <row r="307" spans="9:13">
+    <row r="307" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I307" s="1"/>
       <c r="M307" s="44"/>
     </row>
-    <row r="308" spans="9:13">
+    <row r="308" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I308" s="1"/>
       <c r="M308" s="44"/>
     </row>
-    <row r="309" spans="9:13">
+    <row r="309" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I309" s="1"/>
       <c r="M309" s="44"/>
     </row>
-    <row r="310" spans="9:13">
+    <row r="310" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I310" s="1"/>
       <c r="M310" s="44"/>
     </row>
-    <row r="311" spans="9:13">
+    <row r="311" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I311" s="1"/>
       <c r="M311" s="44"/>
     </row>
-    <row r="312" spans="9:13">
+    <row r="312" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I312" s="1"/>
       <c r="M312" s="44"/>
     </row>
-    <row r="313" spans="9:13">
+    <row r="313" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I313" s="1"/>
     </row>
-    <row r="314" spans="9:13">
+    <row r="314" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I314" s="1"/>
     </row>
-    <row r="315" spans="9:13">
+    <row r="315" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I315" s="1"/>
     </row>
-    <row r="316" spans="9:13">
+    <row r="316" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I316" s="1"/>
     </row>
-    <row r="317" spans="9:13">
+    <row r="317" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I317" s="1"/>
     </row>
-    <row r="318" spans="9:13">
+    <row r="318" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I318" s="1"/>
     </row>
-    <row r="319" spans="9:13">
+    <row r="319" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I319" s="1"/>
     </row>
-    <row r="320" spans="9:13">
+    <row r="320" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I320" s="1"/>
     </row>
-    <row r="321" spans="9:9">
+    <row r="321" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I321" s="1"/>
     </row>
-    <row r="322" spans="9:9">
+    <row r="322" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I322" s="1"/>
     </row>
-    <row r="323" spans="9:9">
+    <row r="323" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I323" s="1"/>
     </row>
-    <row r="324" spans="9:9">
+    <row r="324" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I324" s="1"/>
     </row>
-    <row r="325" spans="9:9">
+    <row r="325" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I325" s="1"/>
     </row>
-    <row r="326" spans="9:9">
+    <row r="326" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I326" s="1"/>
     </row>
-    <row r="327" spans="9:9">
+    <row r="327" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I327" s="1"/>
     </row>
-    <row r="328" spans="9:9">
+    <row r="328" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I328" s="1"/>
     </row>
-    <row r="329" spans="9:9">
+    <row r="329" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I329" s="1"/>
     </row>
-    <row r="330" spans="9:9">
+    <row r="330" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I330" s="1"/>
     </row>
-    <row r="331" spans="9:9">
+    <row r="331" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I331" s="1"/>
     </row>
-    <row r="332" spans="9:9">
+    <row r="332" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I332" s="1"/>
     </row>
-    <row r="333" spans="9:9">
+    <row r="333" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I333" s="1"/>
     </row>
-    <row r="334" spans="9:9">
+    <row r="334" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I334" s="1"/>
     </row>
-    <row r="335" spans="9:9">
+    <row r="335" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I335" s="1"/>
     </row>
-    <row r="336" spans="9:9">
+    <row r="336" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I336" s="1"/>
     </row>
-    <row r="337" spans="9:9">
+    <row r="337" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I337" s="1"/>
     </row>
-    <row r="338" spans="9:9">
+    <row r="338" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I338" s="1"/>
     </row>
-    <row r="339" spans="9:9">
+    <row r="339" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I339" s="1"/>
     </row>
-    <row r="340" spans="9:9">
+    <row r="340" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I340" s="1"/>
     </row>
-    <row r="341" spans="9:9">
+    <row r="341" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I341" s="1"/>
     </row>
-    <row r="342" spans="9:9">
+    <row r="342" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I342" s="1"/>
     </row>
-    <row r="343" spans="9:9">
+    <row r="343" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I343" s="1"/>
     </row>
-    <row r="344" spans="9:9">
+    <row r="344" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I344" s="1"/>
     </row>
-    <row r="345" spans="9:9">
+    <row r="345" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I345" s="1"/>
     </row>
-    <row r="346" spans="9:9">
+    <row r="346" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I346" s="1"/>
     </row>
-    <row r="347" spans="9:9">
+    <row r="347" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I347" s="1"/>
     </row>
-    <row r="348" spans="9:9">
+    <row r="348" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I348" s="1"/>
     </row>
-    <row r="349" spans="9:9">
+    <row r="349" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I349" s="1"/>
     </row>
-    <row r="350" spans="9:9">
+    <row r="350" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I350" s="1"/>
     </row>
-    <row r="351" spans="9:9">
+    <row r="351" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I351" s="1"/>
     </row>
-    <row r="352" spans="9:9">
+    <row r="352" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I352" s="1"/>
     </row>
-    <row r="353" spans="9:9">
+    <row r="353" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I353" s="1"/>
     </row>
-    <row r="354" spans="9:9">
+    <row r="354" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I354" s="1"/>
     </row>
-    <row r="355" spans="9:9">
+    <row r="355" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I355" s="1"/>
     </row>
-    <row r="356" spans="9:9">
+    <row r="356" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I356" s="1"/>
     </row>
-    <row r="357" spans="9:9">
+    <row r="357" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I357" s="1"/>
     </row>
-    <row r="358" spans="9:9">
+    <row r="358" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I358" s="1"/>
     </row>
-    <row r="359" spans="9:9">
+    <row r="359" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I359" s="1"/>
     </row>
-    <row r="360" spans="9:9">
+    <row r="360" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I360" s="1"/>
     </row>
-    <row r="361" spans="9:9">
+    <row r="361" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I361" s="1"/>
     </row>
-    <row r="362" spans="9:9">
+    <row r="362" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I362" s="1"/>
     </row>
-    <row r="363" spans="9:9">
+    <row r="363" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I363" s="1"/>
     </row>
-    <row r="364" spans="9:9">
+    <row r="364" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I364" s="1"/>
     </row>
-    <row r="365" spans="9:9">
+    <row r="365" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I365" s="1"/>
     </row>
-    <row r="366" spans="9:9">
+    <row r="366" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I366" s="1"/>
     </row>
-    <row r="367" spans="9:9">
+    <row r="367" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I367" s="1"/>
     </row>
-    <row r="368" spans="9:9">
+    <row r="368" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I368" s="1"/>
     </row>
-    <row r="369" spans="9:9">
+    <row r="369" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I369" s="1"/>
     </row>
-    <row r="370" spans="9:9">
+    <row r="370" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I370" s="1"/>
     </row>
-    <row r="371" spans="9:9">
+    <row r="371" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I371" s="1"/>
     </row>
-    <row r="372" spans="9:9">
+    <row r="372" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I372" s="1"/>
     </row>
-    <row r="373" spans="9:9">
+    <row r="373" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I373" s="1"/>
     </row>
-    <row r="374" spans="9:9">
+    <row r="374" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I374" s="1"/>
     </row>
-    <row r="375" spans="9:9">
+    <row r="375" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I375" s="1"/>
     </row>
-    <row r="376" spans="9:9">
+    <row r="376" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I376" s="1"/>
     </row>
-    <row r="377" spans="9:9">
+    <row r="377" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I377" s="1"/>
     </row>
-    <row r="378" spans="9:9">
+    <row r="378" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I378" s="1"/>
     </row>
-    <row r="379" spans="9:9">
+    <row r="379" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I379" s="1"/>
     </row>
-    <row r="380" spans="9:9">
+    <row r="380" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I380" s="1"/>
     </row>
-    <row r="381" spans="9:9">
+    <row r="381" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I381" s="1"/>
     </row>
-    <row r="382" spans="9:9">
+    <row r="382" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I382" s="1"/>
     </row>
-    <row r="383" spans="9:9">
+    <row r="383" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I383" s="1"/>
     </row>
   </sheetData>
@@ -7123,12 +7128,12 @@
       <selection activeCell="R69" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="112"/>
+    <col min="1" max="16384" width="8.85546875" style="112"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="112">
         <v>-0.102899</v>
       </c>
@@ -7241,7 +7246,7 @@
         <v>4.7835000000000003E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="112">
         <v>-9.2008999999999994E-2</v>
       </c>
@@ -7354,7 +7359,7 @@
         <v>3.9530999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="112">
         <v>-7.9813999999999996E-2</v>
       </c>
@@ -7467,7 +7472,7 @@
         <v>3.2724000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="112">
         <v>-6.7954000000000001E-2</v>
       </c>
@@ -7580,7 +7585,7 @@
         <v>2.6221999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="112">
         <v>-6.1304999999999998E-2</v>
       </c>
@@ -7693,7 +7698,7 @@
         <v>2.1964000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="112">
         <v>-5.5215E-2</v>
       </c>
@@ -7806,7 +7811,7 @@
         <v>1.8523999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="112">
         <v>-5.0608E-2</v>
       </c>
@@ -7919,7 +7924,7 @@
         <v>1.6164999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="112">
         <v>-4.7326E-2</v>
       </c>
@@ -8032,7 +8037,7 @@
         <v>1.4739E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="112">
         <v>-4.3756999999999997E-2</v>
       </c>
@@ -8145,7 +8150,7 @@
         <v>1.3438E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="112">
         <v>-3.9752000000000003E-2</v>
       </c>
@@ -8258,7 +8263,7 @@
         <v>1.2238000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="112">
         <v>-3.6818999999999998E-2</v>
       </c>
@@ -8371,7 +8376,7 @@
         <v>1.142E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="112">
         <v>-3.4412999999999999E-2</v>
       </c>
@@ -8484,7 +8489,7 @@
         <v>1.0888999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="112">
         <v>-3.1092000000000002E-2</v>
       </c>
@@ -8597,7 +8602,7 @@
         <v>1.0203E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="112">
         <v>-2.8393000000000002E-2</v>
       </c>
@@ -8710,7 +8715,7 @@
         <v>9.6659999999999992E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="112">
         <v>-2.5759000000000001E-2</v>
       </c>
@@ -8823,7 +8828,7 @@
         <v>9.2280000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="112">
         <v>-2.3243E-2</v>
       </c>
@@ -8936,7 +8941,7 @@
         <v>8.7810000000000006E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="112">
         <v>-2.1659000000000001E-2</v>
       </c>
@@ -9049,7 +9054,7 @@
         <v>8.4130000000000003E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="112">
         <v>-2.0065E-2</v>
       </c>
@@ -9162,7 +9167,7 @@
         <v>8.1679999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="112">
         <v>-1.8825999999999999E-2</v>
       </c>
@@ -9275,7 +9280,7 @@
         <v>7.8960000000000002E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="112">
         <v>-1.8134000000000001E-2</v>
       </c>
@@ -9388,7 +9393,7 @@
         <v>7.6779999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="112">
         <v>-1.721E-2</v>
       </c>
@@ -9501,7 +9506,7 @@
         <v>7.476E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="112">
         <v>-1.6492E-2</v>
       </c>
@@ -9614,7 +9619,7 @@
         <v>7.2880000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="112">
         <v>-1.5685999999999999E-2</v>
       </c>
@@ -9727,7 +9732,7 @@
         <v>7.1419999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="112">
         <v>-1.5132E-2</v>
       </c>
@@ -9840,7 +9845,7 @@
         <v>6.9940000000000002E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="112">
         <v>-1.4701000000000001E-2</v>
       </c>
@@ -9953,7 +9958,7 @@
         <v>6.9109999999999996E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="112">
         <v>-1.4076999999999999E-2</v>
       </c>
@@ -10066,7 +10071,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="112">
         <v>-1.3455999999999999E-2</v>
       </c>
@@ -10179,7 +10184,7 @@
         <v>6.7759999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="112">
         <v>-1.311E-2</v>
       </c>
@@ -10292,7 +10297,7 @@
         <v>6.711E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="112">
         <v>-1.2841999999999999E-2</v>
       </c>
@@ -10405,7 +10410,7 @@
         <v>6.6509999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="112">
         <v>-1.2413E-2</v>
       </c>
@@ -10518,7 +10523,7 @@
         <v>6.6119999999999998E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="112">
         <v>-1.2324E-2</v>
       </c>
@@ -10631,7 +10636,7 @@
         <v>6.5160000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="112">
         <v>-1.2546E-2</v>
       </c>
@@ -10744,7 +10749,7 @@
         <v>6.4590000000000003E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="112">
         <v>-1.2839E-2</v>
       </c>
@@ -10857,7 +10862,7 @@
         <v>6.3359999999999996E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="112">
         <v>-1.2834E-2</v>
       </c>
@@ -10970,7 +10975,7 @@
         <v>6.1939999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="112">
         <v>-1.2711E-2</v>
       </c>
@@ -11083,7 +11088,7 @@
         <v>6.0239999999999998E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="112">
         <v>-1.2652999999999999E-2</v>
       </c>
@@ -11196,7 +11201,7 @@
         <v>5.7939999999999997E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="112">
         <v>-1.2411E-2</v>
       </c>
@@ -11309,7 +11314,7 @@
         <v>5.5750000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="112">
         <v>-1.2128999999999999E-2</v>
       </c>
@@ -11422,7 +11427,7 @@
         <v>5.3619999999999996E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="112">
         <v>-1.1508000000000001E-2</v>
       </c>
@@ -11535,7 +11540,7 @@
         <v>5.0720000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="112">
         <v>-1.1006999999999999E-2</v>
       </c>
@@ -11648,7 +11653,7 @@
         <v>4.8349999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="112">
         <v>-1.0260999999999999E-2</v>
       </c>
@@ -11761,7 +11766,7 @@
         <v>4.5909999999999996E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="112">
         <v>-9.6329999999999992E-3</v>
       </c>
@@ -11874,7 +11879,7 @@
         <v>4.2880000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="112">
         <v>-6.2719999999999998E-3</v>
       </c>
@@ -11987,7 +11992,7 @@
         <v>3.4619999999999998E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="112">
         <v>-6.1310000000000002E-3</v>
       </c>
@@ -12100,7 +12105,7 @@
         <v>2.954E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="112">
         <v>-6.0780000000000001E-3</v>
       </c>
@@ -12213,7 +12218,7 @@
         <v>2.5560000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="112">
         <v>-6.0359999999999997E-3</v>
       </c>
@@ -12326,7 +12331,7 @@
         <v>2.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="112">
         <v>-6.0520000000000001E-3</v>
       </c>
@@ -12439,7 +12444,7 @@
         <v>1.949E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="112">
         <v>-6.1879999999999999E-3</v>
       </c>
@@ -12552,7 +12557,7 @@
         <v>1.7060000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="112">
         <v>-6.0670000000000003E-3</v>
       </c>
@@ -12665,7 +12670,7 @@
         <v>1.601E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="112">
         <v>-6.2570000000000004E-3</v>
       </c>
@@ -12778,7 +12783,7 @@
         <v>1.523E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="112">
         <v>-6.3619999999999996E-3</v>
       </c>
@@ -12891,7 +12896,7 @@
         <v>1.4580000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="112">
         <v>-6.1390000000000004E-3</v>
       </c>
@@ -13004,7 +13009,7 @@
         <v>1.526E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="112">
         <v>-6.3169999999999997E-3</v>
       </c>
@@ -13117,7 +13122,7 @@
         <v>1.604E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="112">
         <v>-6.2379999999999996E-3</v>
       </c>
@@ -13230,7 +13235,7 @@
         <v>1.6559999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="112">
         <v>-6.2310000000000004E-3</v>
       </c>
@@ -13343,7 +13348,7 @@
         <v>1.787E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="112">
         <v>-6.3379999999999999E-3</v>
       </c>
@@ -13456,7 +13461,7 @@
         <v>1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="112">
         <v>-6.2969999999999996E-3</v>
       </c>
@@ -13569,7 +13574,7 @@
         <v>1.952E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="112">
         <v>-6.1679999999999999E-3</v>
       </c>
@@ -13682,7 +13687,7 @@
         <v>2.1189999999999998E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="112">
         <v>-6.3819999999999997E-3</v>
       </c>
@@ -13795,7 +13800,7 @@
         <v>2.186E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="112">
         <v>-6.4989999999999996E-3</v>
       </c>
@@ -13908,7 +13913,7 @@
         <v>2.313E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="112">
         <v>-6.5680000000000001E-3</v>
       </c>
@@ -14021,7 +14026,7 @@
         <v>2.4260000000000002E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="112">
         <v>-6.5700000000000003E-3</v>
       </c>
@@ -14134,7 +14139,7 @@
         <v>2.539E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="112">
         <v>-6.4590000000000003E-3</v>
       </c>
@@ -14247,7 +14252,7 @@
         <v>2.5969999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="112">
         <v>-6.4390000000000003E-3</v>
       </c>
@@ -14360,7 +14365,7 @@
         <v>2.7750000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" s="112">
         <v>-6.7149999999999996E-3</v>
       </c>
@@ -14473,7 +14478,7 @@
         <v>2.921E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:37">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" s="112">
         <v>-6.7669999999999996E-3</v>
       </c>
@@ -14586,7 +14591,7 @@
         <v>3.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:37">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" s="112">
         <v>-6.8799999999999998E-3</v>
       </c>
@@ -14699,7 +14704,7 @@
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:37">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" s="112">
         <v>-6.6959999999999997E-3</v>
       </c>
@@ -14812,7 +14817,7 @@
         <v>3.3240000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:37">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" s="112">
         <v>-6.7229999999999998E-3</v>
       </c>
@@ -14925,7 +14930,7 @@
         <v>3.3570000000000002E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:37">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" s="112">
         <v>-6.3749999999999996E-3</v>
       </c>
@@ -15038,7 +15043,7 @@
         <v>3.4380000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:37">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71" s="112">
         <v>-6.6249999999999998E-3</v>
       </c>
@@ -15151,7 +15156,7 @@
         <v>3.4480000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:37">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" s="112">
         <v>-6.1219999999999998E-3</v>
       </c>
@@ -15264,7 +15269,7 @@
         <v>3.444E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" s="112">
         <v>-5.9829999999999996E-3</v>
       </c>
@@ -15377,7 +15382,7 @@
         <v>3.4889999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:37">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" s="112">
         <v>-6.0089999999999996E-3</v>
       </c>
@@ -15490,7 +15495,7 @@
         <v>3.3140000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:37">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" s="112">
         <v>-5.5570000000000003E-3</v>
       </c>
@@ -15603,7 +15608,7 @@
         <v>3.3110000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:37">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" s="112">
         <v>-5.7099999999999998E-3</v>
       </c>
@@ -15716,7 +15721,7 @@
         <v>3.2759999999999998E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:37">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" s="112">
         <v>-5.7060000000000001E-3</v>
       </c>
@@ -15829,7 +15834,7 @@
         <v>3.1220000000000002E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37">
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78" s="112">
         <v>-5.5230000000000001E-3</v>
       </c>
@@ -15942,7 +15947,7 @@
         <v>2.993E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" s="112">
         <v>-5.4010000000000004E-3</v>
       </c>
@@ -16055,7 +16060,7 @@
         <v>3.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:37">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80" s="112">
         <v>-5.8849999999999996E-3</v>
       </c>
@@ -16168,7 +16173,7 @@
         <v>3.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:37">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A81" s="112">
         <v>-5.5620000000000001E-3</v>
       </c>
@@ -16281,7 +16286,7 @@
         <v>3.0230000000000001E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:37">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" s="112">
         <v>-5.6230000000000004E-3</v>
       </c>
@@ -16394,7 +16399,7 @@
         <v>2.9949999999999998E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A83" s="112">
         <v>-5.594E-3</v>
       </c>
@@ -16525,12 +16530,12 @@
       <selection activeCell="AK83" sqref="AK83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.83203125" style="112"/>
+    <col min="1" max="16384" width="8.85546875" style="112"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="112">
         <v>1.7951000000000002E-2</v>
       </c>
@@ -16643,7 +16648,7 @@
         <v>-1.6435000000000002E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="112">
         <v>1.2437E-2</v>
       </c>
@@ -16756,7 +16761,7 @@
         <v>-1.3527000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="112">
         <v>5.5900000000000004E-3</v>
       </c>
@@ -16869,7 +16874,7 @@
         <v>-1.1609E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="112">
         <v>2.441E-3</v>
       </c>
@@ -16982,7 +16987,7 @@
         <v>-9.3799999999999994E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="112">
         <v>3.0769999999999999E-3</v>
       </c>
@@ -17095,7 +17100,7 @@
         <v>-7.8279999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="112">
         <v>-1.7229999999999999E-3</v>
       </c>
@@ -17208,7 +17213,7 @@
         <v>-7.2960000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="112">
         <v>-1.639E-3</v>
       </c>
@@ -17321,7 +17326,7 @@
         <v>-5.6899999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="112">
         <v>-3.9490000000000003E-3</v>
       </c>
@@ -17434,7 +17439,7 @@
         <v>-5.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="112">
         <v>-5.091E-3</v>
       </c>
@@ -17547,7 +17552,7 @@
         <v>-4.3169999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="112">
         <v>-6.2509999999999996E-3</v>
       </c>
@@ -17660,7 +17665,7 @@
         <v>-3.8920000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="112">
         <v>-7.6689999999999996E-3</v>
       </c>
@@ -17773,7 +17778,7 @@
         <v>-3.3760000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="112">
         <v>-7.5690000000000002E-3</v>
       </c>
@@ -17886,7 +17891,7 @@
         <v>-2.9299999999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="112">
         <v>-7.8449999999999995E-3</v>
       </c>
@@ -17999,7 +18004,7 @@
         <v>-2.6180000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="112">
         <v>-8.1080000000000006E-3</v>
       </c>
@@ -18112,7 +18117,7 @@
         <v>-2.1870000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" s="112">
         <v>-8.1810000000000008E-3</v>
       </c>
@@ -18225,7 +18230,7 @@
         <v>-2.0899999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="112">
         <v>-7.0410000000000004E-3</v>
       </c>
@@ -18338,7 +18343,7 @@
         <v>-1.684E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="112">
         <v>-7.5420000000000001E-3</v>
       </c>
@@ -18451,7 +18456,7 @@
         <v>-1.601E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="112">
         <v>-6.7739999999999996E-3</v>
       </c>
@@ -18564,7 +18569,7 @@
         <v>-1.341E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="112">
         <v>-5.7710000000000001E-3</v>
       </c>
@@ -18677,7 +18682,7 @@
         <v>-1.013E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="112">
         <v>-6.5979999999999997E-3</v>
       </c>
@@ -18790,7 +18795,7 @@
         <v>-1.0449999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="112">
         <v>-5.731E-3</v>
       </c>
@@ -18903,7 +18908,7 @@
         <v>-7.9299999999999998E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="112">
         <v>-5.2379999999999996E-3</v>
       </c>
@@ -19016,7 +19021,7 @@
         <v>-5.4199999999999995E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A23" s="112">
         <v>-5.9519999999999998E-3</v>
       </c>
@@ -19129,7 +19134,7 @@
         <v>-6.0300000000000002E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A24" s="112">
         <v>-5.2240000000000003E-3</v>
       </c>
@@ -19242,7 +19247,7 @@
         <v>-5.0199999999999995E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="112">
         <v>-4.816E-3</v>
       </c>
@@ -19355,7 +19360,7 @@
         <v>-2.8699999999999998E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A26" s="112">
         <v>-5.1489999999999999E-3</v>
       </c>
@@ -19468,7 +19473,7 @@
         <v>-2.9300000000000002E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A27" s="112">
         <v>-4.5799999999999999E-3</v>
       </c>
@@ -19581,7 +19586,7 @@
         <v>-1.8799999999999999E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="112">
         <v>-3.9309999999999996E-3</v>
       </c>
@@ -19694,7 +19699,7 @@
         <v>-8.2999999999999998E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="112">
         <v>-4.3629999999999997E-3</v>
       </c>
@@ -19807,7 +19812,7 @@
         <v>-4.1999999999999998E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="112">
         <v>-3.0850000000000001E-3</v>
       </c>
@@ -19920,7 +19925,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="112">
         <v>-3.1389999999999999E-3</v>
       </c>
@@ -20033,7 +20038,7 @@
         <v>2.1499999999999999E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A32" s="112">
         <v>-3.1210000000000001E-3</v>
       </c>
@@ -20146,7 +20151,7 @@
         <v>1.9100000000000001E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A33" s="112">
         <v>-2.4740000000000001E-3</v>
       </c>
@@ -20259,7 +20264,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="112">
         <v>-2.5569999999999998E-3</v>
       </c>
@@ -20372,7 +20377,7 @@
         <v>4.2299999999999998E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="112">
         <v>-2.9510000000000001E-3</v>
       </c>
@@ -20485,7 +20490,7 @@
         <v>3.68E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A36" s="112">
         <v>-2.545E-3</v>
       </c>
@@ -20598,7 +20603,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A37" s="112">
         <v>-2.5179999999999998E-3</v>
       </c>
@@ -20711,7 +20716,7 @@
         <v>4.0099999999999999E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A38" s="112">
         <v>-2.8119999999999998E-3</v>
       </c>
@@ -20824,7 +20829,7 @@
         <v>3.6900000000000002E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A39" s="112">
         <v>-2.5339999999999998E-3</v>
       </c>
@@ -20937,7 +20942,7 @@
         <v>3.57E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A40" s="112">
         <v>-2.5709999999999999E-3</v>
       </c>
@@ -21050,7 +21055,7 @@
         <v>2.13E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A41" s="112">
         <v>-1.9480000000000001E-3</v>
       </c>
@@ -21163,7 +21168,7 @@
         <v>5.8E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A42" s="112">
         <v>-2.0049999999999998E-3</v>
       </c>
@@ -21276,7 +21281,7 @@
         <v>-7.4999999999999993E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A43" s="112">
         <v>-1.8489999999999999E-3</v>
       </c>
@@ -21389,7 +21394,7 @@
         <v>-3.48E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A44" s="112">
         <v>-1.8420000000000001E-3</v>
       </c>
@@ -21502,7 +21507,7 @@
         <v>-4.9799999999999996E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A45" s="112">
         <v>-1.792E-3</v>
       </c>
@@ -21615,7 +21620,7 @@
         <v>-8.0900000000000004E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A46" s="112">
         <v>-1.946E-3</v>
       </c>
@@ -21728,7 +21733,7 @@
         <v>-9.3700000000000001E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A47" s="112">
         <v>-1.89E-3</v>
       </c>
@@ -21841,7 +21846,7 @@
         <v>-1.034E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A48" s="112">
         <v>-1.9959999999999999E-3</v>
       </c>
@@ -21954,7 +21959,7 @@
         <v>-1.294E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A49" s="112">
         <v>-2.1489999999999999E-3</v>
       </c>
@@ -22067,7 +22072,7 @@
         <v>-1.457E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A50" s="112">
         <v>-1.9120000000000001E-3</v>
       </c>
@@ -22180,7 +22185,7 @@
         <v>-1.523E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A51" s="112">
         <v>-1.7960000000000001E-3</v>
       </c>
@@ -22293,7 +22298,7 @@
         <v>-1.642E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A52" s="112">
         <v>-1.7769999999999999E-3</v>
       </c>
@@ -22406,7 +22411,7 @@
         <v>-1.5770000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A53" s="112">
         <v>-1.918E-3</v>
       </c>
@@ -22519,7 +22524,7 @@
         <v>-1.8879999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A54" s="112">
         <v>-1.3630000000000001E-3</v>
       </c>
@@ -22632,7 +22637,7 @@
         <v>-1.784E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A55" s="112">
         <v>-1.34E-3</v>
       </c>
@@ -22745,7 +22750,7 @@
         <v>-1.835E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A56" s="112">
         <v>-1.142E-3</v>
       </c>
@@ -22858,7 +22863,7 @@
         <v>-1.885E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A57" s="112">
         <v>-7.5900000000000002E-4</v>
       </c>
@@ -22971,7 +22976,7 @@
         <v>-1.946E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A58" s="112">
         <v>-6.1399999999999996E-4</v>
       </c>
@@ -23084,7 +23089,7 @@
         <v>-1.946E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A59" s="112">
         <v>-4.7800000000000002E-4</v>
       </c>
@@ -23197,7 +23202,7 @@
         <v>-1.902E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A60" s="112">
         <v>-8.1000000000000004E-5</v>
       </c>
@@ -23310,7 +23315,7 @@
         <v>-1.9620000000000002E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A61" s="112">
         <v>-6.3E-5</v>
       </c>
@@ -23423,7 +23428,7 @@
         <v>-1.8990000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A62" s="112">
         <v>-1.2999999999999999E-5</v>
       </c>
@@ -23536,7 +23541,7 @@
         <v>-1.882E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A63" s="112">
         <v>2.02E-4</v>
       </c>
@@ -23649,7 +23654,7 @@
         <v>-1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A64" s="112">
         <v>-1.2999999999999999E-4</v>
       </c>
@@ -23762,7 +23767,7 @@
         <v>-1.867E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37">
+    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A65" s="112">
         <v>-3.4200000000000002E-4</v>
       </c>
@@ -23875,7 +23880,7 @@
         <v>-1.8309999999999999E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:37">
+    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A66" s="112">
         <v>-4.3999999999999999E-5</v>
       </c>
@@ -23988,7 +23993,7 @@
         <v>-1.622E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:37">
+    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A67" s="112">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -24101,7 +24106,7 @@
         <v>-1.689E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:37">
+    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A68" s="112">
         <v>-1.7100000000000001E-4</v>
       </c>
@@ -24214,7 +24219,7 @@
         <v>-1.5870000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:37">
+    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A69" s="112">
         <v>1.15E-4</v>
       </c>
@@ -24327,7 +24332,7 @@
         <v>-1.482E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:37">
+    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A70" s="112">
         <v>1.02E-4</v>
       </c>
@@ -24440,7 +24445,7 @@
         <v>-1.3519999999999999E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:37">
+    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A71" s="112">
         <v>9.0000000000000006E-5</v>
       </c>
@@ -24553,7 +24558,7 @@
         <v>-1.2049999999999999E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:37">
+    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A72" s="112">
         <v>7.0699999999999995E-4</v>
       </c>
@@ -24666,7 +24671,7 @@
         <v>-1.191E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37">
+    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A73" s="112">
         <v>4.6200000000000001E-4</v>
       </c>
@@ -24779,7 +24784,7 @@
         <v>-1.1100000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:37">
+    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A74" s="112">
         <v>1.178E-3</v>
       </c>
@@ -24892,7 +24897,7 @@
         <v>-1.1820000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:37">
+    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A75" s="112">
         <v>1.0859999999999999E-3</v>
       </c>
@@ -25005,7 +25010,7 @@
         <v>-1.0939999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:37">
+    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A76" s="112">
         <v>1.1479999999999999E-3</v>
       </c>
@@ -25118,7 +25123,7 @@
         <v>-1.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:37">
+    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A77" s="112">
         <v>1.6659999999999999E-3</v>
       </c>
@@ -25231,7 +25236,7 @@
         <v>-1.0889999999999999E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37">
+    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A78" s="112">
         <v>1.645E-3</v>
       </c>
@@ -25344,7 +25349,7 @@
         <v>-1.2639999999999999E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37">
+    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A79" s="112">
         <v>1.446E-3</v>
       </c>
@@ -25457,7 +25462,7 @@
         <v>-1.175E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:37">
+    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A80" s="112">
         <v>1.7979999999999999E-3</v>
       </c>
@@ -25570,7 +25575,7 @@
         <v>-1.2800000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:37">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A81" s="112">
         <v>1.81E-3</v>
       </c>
@@ -25683,7 +25688,7 @@
         <v>-1.4220000000000001E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:37">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A82" s="112">
         <v>1.4289999999999999E-3</v>
       </c>
@@ -25796,7 +25801,7 @@
         <v>-1.397E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A83" s="112">
         <v>2.15E-3</v>
       </c>

</xml_diff>

<commit_message>
Pioneer moorings - fixed deployment dates
Fixed deployment dates based on cruise reports and WHOI documentation
</commit_message>
<xml_diff>
--- a/deployment/Omaha_Cal_Info_CP01CNSM_00004.xlsx
+++ b/deployment/Omaha_Cal_Info_CP01CNSM_00004.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AST1799\Documents\OOI\OOI Douments\CI\asset-management\deployment\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="1395" windowWidth="20730" windowHeight="11760" tabRatio="766" activeTab="1"/>
+    <workbookView xWindow="12340" yWindow="2200" windowWidth="20740" windowHeight="11760" tabRatio="766"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="2" r:id="rId1"/>
@@ -24,7 +19,7 @@
     <definedName name="_FilterDatabase_0">[1]Moorings!#REF!</definedName>
     <definedName name="_FilterDatabase_0_0_0">[1]Moorings!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1808,7 +1803,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Read Me"/>
@@ -1867,7 +1862,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1902,7 +1897,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2113,28 +2108,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="61" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" style="61" customWidth="1"/>
     <col min="2" max="2" width="16" style="61" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" style="61" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="61" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="62" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="63" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="62" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="61" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="61" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" style="61" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="61" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.7109375" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" style="61" customWidth="1"/>
+    <col min="5" max="5" width="11.5" style="62" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="63" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="62" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" style="61" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="61" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" style="61" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" style="61" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" style="61" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="61"/>
+    <col min="14" max="14" width="12.6640625" style="61" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="58" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="58" customFormat="1" ht="28">
       <c r="A1" s="53" t="s">
         <v>151</v>
       </c>
@@ -2172,7 +2169,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="61" t="s">
         <v>152</v>
       </c>
@@ -2191,7 +2188,9 @@
       <c r="F2" s="65">
         <v>0.78472222222222221</v>
       </c>
-      <c r="G2" s="60"/>
+      <c r="G2" s="60">
+        <v>42464</v>
+      </c>
       <c r="H2" s="11" t="s">
         <v>133</v>
       </c>
@@ -2214,8 +2213,8 @@
         <v>-70.778433333333339</v>
       </c>
     </row>
-    <row r="4" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:14" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:14" customFormat="1"/>
+    <row r="5" spans="1:14" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2231,31 +2230,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V383"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="44" customWidth="1"/>
+    <col min="1" max="1" width="30.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="44" customWidth="1"/>
     <col min="3" max="3" width="17" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="45" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="8" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="1"/>
-    <col min="11" max="11" width="4.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="45" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.33203125" style="8" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="1"/>
+    <col min="11" max="11" width="4.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="1" customWidth="1"/>
     <col min="14" max="14" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="1"/>
+    <col min="15" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="7" customFormat="1" ht="28">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2288,7 +2287,7 @@
       <c r="L1" s="36"/>
       <c r="M1" s="36"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18">
       <c r="C2" s="18"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -2296,7 +2295,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -2319,7 +2318,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" s="44" customFormat="1">
       <c r="A4" s="42"/>
       <c r="B4" s="42"/>
       <c r="C4" s="17"/>
@@ -2329,7 +2328,7 @@
       <c r="G4" s="41"/>
       <c r="H4" s="41"/>
     </row>
-    <row r="5" spans="1:18" s="73" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" s="73" customFormat="1">
       <c r="A5" s="89" t="s">
         <v>114</v>
       </c>
@@ -2354,7 +2353,7 @@
       <c r="M5" s="44"/>
       <c r="R5" s="44"/>
     </row>
-    <row r="6" spans="1:18" s="73" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" s="73" customFormat="1">
       <c r="A6" s="89" t="s">
         <v>115</v>
       </c>
@@ -2379,12 +2378,12 @@
       <c r="M6" s="44"/>
       <c r="R6" s="44"/>
     </row>
-    <row r="7" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" s="44" customFormat="1">
       <c r="C7" s="42"/>
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
     </row>
-    <row r="8" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -2413,7 +2412,7 @@
       <c r="M8" s="44"/>
       <c r="R8" s="44"/>
     </row>
-    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2442,7 +2441,7 @@
       <c r="M9" s="44"/>
       <c r="R9" s="44"/>
     </row>
-    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -2471,7 +2470,7 @@
       <c r="M10" s="44"/>
       <c r="R10" s="44"/>
     </row>
-    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -2500,7 +2499,7 @@
       <c r="M11" s="44"/>
       <c r="R11" s="44"/>
     </row>
-    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -2529,7 +2528,7 @@
       <c r="M12" s="44"/>
       <c r="R12" s="44"/>
     </row>
-    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -2558,7 +2557,7 @@
       <c r="M13" s="44"/>
       <c r="R13" s="44"/>
     </row>
-    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -2589,7 +2588,7 @@
       <c r="M14" s="44"/>
       <c r="R14" s="44"/>
     </row>
-    <row r="15" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -2620,7 +2619,7 @@
       <c r="M15" s="44"/>
       <c r="R15" s="44"/>
     </row>
-    <row r="16" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18">
       <c r="A16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2651,7 +2650,7 @@
       <c r="M16" s="44"/>
       <c r="R16" s="44"/>
     </row>
-    <row r="17" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" s="44" customFormat="1">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
       <c r="C17" s="17"/>
@@ -2661,7 +2660,7 @@
       <c r="G17" s="41"/>
       <c r="H17" s="41"/>
     </row>
-    <row r="18" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -2690,7 +2689,7 @@
       <c r="M18" s="44"/>
       <c r="R18" s="44"/>
     </row>
-    <row r="19" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18">
       <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
@@ -2719,7 +2718,7 @@
       <c r="M19" s="44"/>
       <c r="R19" s="44"/>
     </row>
-    <row r="20" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -2748,7 +2747,7 @@
       <c r="M20" s="44"/>
       <c r="R20" s="44"/>
     </row>
-    <row r="21" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
@@ -2777,7 +2776,7 @@
       <c r="M21" s="44"/>
       <c r="R21" s="44"/>
     </row>
-    <row r="22" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -2806,7 +2805,7 @@
       <c r="M22" s="44"/>
       <c r="R22" s="44"/>
     </row>
-    <row r="23" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -2835,7 +2834,7 @@
       <c r="M23" s="44"/>
       <c r="R23" s="44"/>
     </row>
-    <row r="24" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -2866,7 +2865,7 @@
       <c r="M24" s="44"/>
       <c r="R24" s="44"/>
     </row>
-    <row r="25" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -2897,7 +2896,7 @@
       <c r="M25" s="44"/>
       <c r="R25" s="44"/>
     </row>
-    <row r="26" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18">
       <c r="A26" s="2" t="s">
         <v>26</v>
       </c>
@@ -2928,7 +2927,7 @@
       <c r="M26" s="44"/>
       <c r="R26" s="44"/>
     </row>
-    <row r="27" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" s="44" customFormat="1">
       <c r="A27" s="42"/>
       <c r="B27" s="42"/>
       <c r="C27" s="17"/>
@@ -2938,7 +2937,7 @@
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
     </row>
-    <row r="28" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -2963,7 +2962,7 @@
       <c r="M28" s="44"/>
       <c r="R28" s="44"/>
     </row>
-    <row r="29" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" s="44" customFormat="1">
       <c r="A29" s="42"/>
       <c r="B29" s="42"/>
       <c r="C29" s="17"/>
@@ -2973,7 +2972,7 @@
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
     </row>
-    <row r="30" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18">
       <c r="A30" s="12" t="s">
         <v>35</v>
       </c>
@@ -3002,7 +3001,7 @@
       <c r="M30" s="44"/>
       <c r="R30" s="44"/>
     </row>
-    <row r="31" spans="1:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18">
       <c r="A31" s="47" t="s">
         <v>35</v>
       </c>
@@ -3031,7 +3030,7 @@
       <c r="M31" s="44"/>
       <c r="R31" s="44"/>
     </row>
-    <row r="32" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" s="44" customFormat="1">
       <c r="A32" s="42"/>
       <c r="B32" s="42"/>
       <c r="C32" s="17"/>
@@ -3041,7 +3040,7 @@
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
     </row>
-    <row r="33" spans="1:18" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" s="44" customFormat="1">
       <c r="A33" s="23" t="s">
         <v>103</v>
       </c>
@@ -3070,7 +3069,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:18" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" s="44" customFormat="1">
       <c r="A34" s="23" t="s">
         <v>103</v>
       </c>
@@ -3094,7 +3093,7 @@
         <v>-70.778433333333339</v>
       </c>
     </row>
-    <row r="35" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" s="44" customFormat="1">
       <c r="A35" s="42"/>
       <c r="B35" s="42"/>
       <c r="C35" s="17"/>
@@ -3104,7 +3103,7 @@
       <c r="G35" s="41"/>
       <c r="H35" s="41"/>
     </row>
-    <row r="36" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18">
       <c r="A36" s="12" t="s">
         <v>36</v>
       </c>
@@ -3133,7 +3132,7 @@
       <c r="M36" s="44"/>
       <c r="R36" s="44"/>
     </row>
-    <row r="37" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18">
       <c r="A37" s="47" t="s">
         <v>36</v>
       </c>
@@ -3161,7 +3160,7 @@
       <c r="I37" s="1"/>
       <c r="M37" s="44"/>
     </row>
-    <row r="38" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" s="44" customFormat="1">
       <c r="A38" s="42"/>
       <c r="B38" s="42"/>
       <c r="C38" s="17"/>
@@ -3171,7 +3170,7 @@
       <c r="G38" s="41"/>
       <c r="H38" s="41"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18">
       <c r="I39" s="12" t="s">
         <v>104</v>
       </c>
@@ -3188,7 +3187,7 @@
       <c r="N39" s="117"/>
       <c r="O39" s="123"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18">
       <c r="I40" s="47" t="s">
         <v>104</v>
       </c>
@@ -3204,7 +3203,7 @@
       <c r="M40" s="44"/>
       <c r="N40" s="118"/>
     </row>
-    <row r="41" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" s="44" customFormat="1">
       <c r="A41" s="42"/>
       <c r="B41" s="42"/>
       <c r="C41" s="17"/>
@@ -3214,7 +3213,7 @@
       <c r="G41" s="41"/>
       <c r="H41" s="41"/>
     </row>
-    <row r="42" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18">
       <c r="I42" s="15" t="s">
         <v>37</v>
       </c>
@@ -3230,7 +3229,7 @@
       <c r="M42" s="44"/>
       <c r="N42" s="94"/>
     </row>
-    <row r="43" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18">
       <c r="I43" s="48" t="s">
         <v>37</v>
       </c>
@@ -3246,7 +3245,7 @@
       <c r="M43" s="44"/>
       <c r="N43" s="94"/>
     </row>
-    <row r="44" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18">
       <c r="I44" s="48" t="s">
         <v>37</v>
       </c>
@@ -3262,7 +3261,7 @@
       <c r="M44" s="44"/>
       <c r="N44" s="94"/>
     </row>
-    <row r="45" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18">
       <c r="I45" s="48" t="s">
         <v>37</v>
       </c>
@@ -3278,7 +3277,7 @@
       <c r="M45" s="44"/>
       <c r="N45" s="94"/>
     </row>
-    <row r="46" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18">
       <c r="I46" s="48" t="s">
         <v>37</v>
       </c>
@@ -3294,7 +3293,7 @@
       <c r="M46" s="44"/>
       <c r="N46" s="95"/>
     </row>
-    <row r="47" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18">
       <c r="I47" s="48" t="s">
         <v>37</v>
       </c>
@@ -3310,7 +3309,7 @@
       <c r="M47" s="44"/>
       <c r="N47" s="95"/>
     </row>
-    <row r="48" spans="1:18" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" s="44" customFormat="1">
       <c r="I48" s="48" t="s">
         <v>37</v>
       </c>
@@ -3325,7 +3324,7 @@
       </c>
       <c r="N48" s="67"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:15">
       <c r="A49" s="18"/>
       <c r="B49" s="42"/>
       <c r="C49" s="17"/>
@@ -3336,7 +3335,7 @@
       <c r="I49" s="1"/>
       <c r="M49" s="44"/>
     </row>
-    <row r="50" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:15">
       <c r="I50" s="15" t="s">
         <v>38</v>
       </c>
@@ -3353,7 +3352,7 @@
       <c r="N50" s="94"/>
       <c r="O50" s="123"/>
     </row>
-    <row r="51" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:15">
       <c r="I51" s="48" t="s">
         <v>38</v>
       </c>
@@ -3369,7 +3368,7 @@
       <c r="M51" s="44"/>
       <c r="N51" s="94"/>
     </row>
-    <row r="52" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:15">
       <c r="I52" s="48" t="s">
         <v>38</v>
       </c>
@@ -3385,7 +3384,7 @@
       <c r="M52" s="44"/>
       <c r="N52" s="94"/>
     </row>
-    <row r="53" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:15">
       <c r="I53" s="48" t="s">
         <v>38</v>
       </c>
@@ -3401,7 +3400,7 @@
       <c r="M53" s="44"/>
       <c r="N53" s="94"/>
     </row>
-    <row r="54" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:15">
       <c r="I54" s="48" t="s">
         <v>38</v>
       </c>
@@ -3417,7 +3416,7 @@
       <c r="M54" s="44"/>
       <c r="N54" s="95"/>
     </row>
-    <row r="55" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:15">
       <c r="I55" s="48" t="s">
         <v>38</v>
       </c>
@@ -3433,7 +3432,7 @@
       <c r="M55" s="44"/>
       <c r="N55" s="95"/>
     </row>
-    <row r="56" spans="1:15" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:15" s="44" customFormat="1">
       <c r="I56" s="48" t="s">
         <v>38</v>
       </c>
@@ -3448,7 +3447,7 @@
       </c>
       <c r="N56" s="67"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:15">
       <c r="A57" s="18"/>
       <c r="B57" s="42"/>
       <c r="C57" s="17"/>
@@ -3459,7 +3458,7 @@
       <c r="I57" s="1"/>
       <c r="M57" s="44"/>
     </row>
-    <row r="58" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:15">
       <c r="A58" s="19" t="s">
         <v>39</v>
       </c>
@@ -3487,7 +3486,7 @@
       <c r="I58" s="1"/>
       <c r="M58" s="44"/>
     </row>
-    <row r="59" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:15">
       <c r="A59" s="49" t="s">
         <v>39</v>
       </c>
@@ -3515,7 +3514,7 @@
       <c r="I59" s="1"/>
       <c r="M59" s="44"/>
     </row>
-    <row r="60" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:15">
       <c r="A60" s="49" t="s">
         <v>39</v>
       </c>
@@ -3543,7 +3542,7 @@
       <c r="I60" s="1"/>
       <c r="M60" s="44"/>
     </row>
-    <row r="61" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:15">
       <c r="A61" s="49" t="s">
         <v>39</v>
       </c>
@@ -3571,7 +3570,7 @@
       <c r="I61" s="1"/>
       <c r="M61" s="44"/>
     </row>
-    <row r="62" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:15">
       <c r="A62" s="49" t="s">
         <v>39</v>
       </c>
@@ -3599,7 +3598,7 @@
       <c r="I62" s="1"/>
       <c r="M62" s="44"/>
     </row>
-    <row r="63" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:15">
       <c r="A63" s="49" t="s">
         <v>39</v>
       </c>
@@ -3627,7 +3626,7 @@
       <c r="I63" s="1"/>
       <c r="M63" s="44"/>
     </row>
-    <row r="64" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:15">
       <c r="A64" s="49" t="s">
         <v>39</v>
       </c>
@@ -3655,7 +3654,7 @@
       <c r="I64" s="1"/>
       <c r="M64" s="44"/>
     </row>
-    <row r="65" spans="1:15" s="21" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:15" s="21" customFormat="1">
       <c r="A65" s="49" t="s">
         <v>39</v>
       </c>
@@ -3682,7 +3681,7 @@
       </c>
       <c r="M65" s="44"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:15">
       <c r="A66" s="18"/>
       <c r="B66" s="42"/>
       <c r="C66" s="17"/>
@@ -3693,7 +3692,7 @@
       <c r="I66" s="1"/>
       <c r="M66" s="44"/>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:15">
       <c r="I67" s="19" t="s">
         <v>40</v>
       </c>
@@ -3710,7 +3709,7 @@
       <c r="N67" s="94"/>
       <c r="O67" s="123"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:15">
       <c r="I68" s="49" t="s">
         <v>40</v>
       </c>
@@ -3726,7 +3725,7 @@
       <c r="M68" s="44"/>
       <c r="N68" s="94"/>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:15">
       <c r="I69" s="49" t="s">
         <v>40</v>
       </c>
@@ -3742,7 +3741,7 @@
       <c r="M69" s="44"/>
       <c r="N69" s="94"/>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:15">
       <c r="I70" s="49" t="s">
         <v>40</v>
       </c>
@@ -3758,7 +3757,7 @@
       <c r="M70" s="44"/>
       <c r="N70" s="94"/>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:15">
       <c r="I71" s="49" t="s">
         <v>40</v>
       </c>
@@ -3774,7 +3773,7 @@
       <c r="M71" s="44"/>
       <c r="N71" s="94"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:15">
       <c r="I72" s="49" t="s">
         <v>40</v>
       </c>
@@ -3790,7 +3789,7 @@
       <c r="M72" s="44"/>
       <c r="N72" s="94"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:15">
       <c r="I73" s="49" t="s">
         <v>40</v>
       </c>
@@ -3806,7 +3805,7 @@
       <c r="M73" s="44"/>
       <c r="N73" s="94"/>
     </row>
-    <row r="74" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:15">
       <c r="I74" s="49" t="s">
         <v>40</v>
       </c>
@@ -3822,7 +3821,7 @@
       <c r="M74" s="44"/>
       <c r="N74" s="94"/>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:15">
       <c r="A75" s="18"/>
       <c r="B75" s="42"/>
       <c r="C75" s="17"/>
@@ -3833,7 +3832,7 @@
       <c r="I75" s="1"/>
       <c r="M75" s="44"/>
     </row>
-    <row r="76" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:15">
       <c r="A76" s="23" t="s">
         <v>43</v>
       </c>
@@ -3861,7 +3860,7 @@
       <c r="I76" s="1"/>
       <c r="M76" s="44"/>
     </row>
-    <row r="77" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:15">
       <c r="A77" s="50" t="s">
         <v>43</v>
       </c>
@@ -3889,7 +3888,7 @@
       <c r="I77" s="1"/>
       <c r="M77" s="44"/>
     </row>
-    <row r="78" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:15">
       <c r="A78" s="50" t="s">
         <v>43</v>
       </c>
@@ -3917,7 +3916,7 @@
       <c r="I78" s="1"/>
       <c r="M78" s="44"/>
     </row>
-    <row r="79" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:15">
       <c r="A79" s="50" t="s">
         <v>43</v>
       </c>
@@ -3945,7 +3944,7 @@
       <c r="I79" s="1"/>
       <c r="M79" s="44"/>
     </row>
-    <row r="80" spans="1:15" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:15">
       <c r="A80" s="50" t="s">
         <v>43</v>
       </c>
@@ -3973,7 +3972,7 @@
       <c r="I80" s="1"/>
       <c r="M80" s="44"/>
     </row>
-    <row r="81" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13">
       <c r="A81" s="50" t="s">
         <v>43</v>
       </c>
@@ -4001,7 +4000,7 @@
       <c r="I81" s="1"/>
       <c r="M81" s="44"/>
     </row>
-    <row r="82" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13">
       <c r="A82" s="50" t="s">
         <v>43</v>
       </c>
@@ -4031,7 +4030,7 @@
       </c>
       <c r="M82" s="44"/>
     </row>
-    <row r="83" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13">
       <c r="A83" s="50" t="s">
         <v>43</v>
       </c>
@@ -4061,7 +4060,7 @@
       </c>
       <c r="M83" s="44"/>
     </row>
-    <row r="84" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13">
       <c r="A84" s="50" t="s">
         <v>43</v>
       </c>
@@ -4091,7 +4090,7 @@
       </c>
       <c r="M84" s="44"/>
     </row>
-    <row r="85" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13">
       <c r="A85" s="50" t="s">
         <v>43</v>
       </c>
@@ -4121,7 +4120,7 @@
       </c>
       <c r="M85" s="44"/>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13">
       <c r="A86" s="18"/>
       <c r="B86" s="42"/>
       <c r="C86" s="17"/>
@@ -4132,7 +4131,7 @@
       <c r="I86" s="1"/>
       <c r="M86" s="44"/>
     </row>
-    <row r="87" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13">
       <c r="A87" s="19" t="s">
         <v>44</v>
       </c>
@@ -4160,7 +4159,7 @@
       <c r="I87" s="1"/>
       <c r="M87" s="44"/>
     </row>
-    <row r="88" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" s="40" customFormat="1">
       <c r="A88" s="49" t="s">
         <v>44</v>
       </c>
@@ -4187,7 +4186,7 @@
       </c>
       <c r="M88" s="44"/>
     </row>
-    <row r="89" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" s="40" customFormat="1">
       <c r="A89" s="49" t="s">
         <v>44</v>
       </c>
@@ -4214,7 +4213,7 @@
       </c>
       <c r="M89" s="44"/>
     </row>
-    <row r="90" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" s="40" customFormat="1">
       <c r="A90" s="49" t="s">
         <v>44</v>
       </c>
@@ -4241,7 +4240,7 @@
       </c>
       <c r="M90" s="44"/>
     </row>
-    <row r="91" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" s="40" customFormat="1">
       <c r="A91" s="49" t="s">
         <v>44</v>
       </c>
@@ -4268,7 +4267,7 @@
       </c>
       <c r="M91" s="44"/>
     </row>
-    <row r="92" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" s="40" customFormat="1">
       <c r="A92" s="49" t="s">
         <v>44</v>
       </c>
@@ -4295,7 +4294,7 @@
       </c>
       <c r="M92" s="44"/>
     </row>
-    <row r="93" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" s="40" customFormat="1">
       <c r="A93" s="49" t="s">
         <v>44</v>
       </c>
@@ -4322,7 +4321,7 @@
       </c>
       <c r="M93" s="44"/>
     </row>
-    <row r="94" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" s="40" customFormat="1">
       <c r="A94" s="49" t="s">
         <v>44</v>
       </c>
@@ -4349,7 +4348,7 @@
       </c>
       <c r="M94" s="44"/>
     </row>
-    <row r="95" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" s="40" customFormat="1">
       <c r="A95" s="49" t="s">
         <v>44</v>
       </c>
@@ -4376,7 +4375,7 @@
       </c>
       <c r="M95" s="44"/>
     </row>
-    <row r="96" spans="1:13" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" s="40" customFormat="1">
       <c r="A96" s="49" t="s">
         <v>44</v>
       </c>
@@ -4403,7 +4402,7 @@
       </c>
       <c r="M96" s="44"/>
     </row>
-    <row r="97" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:15" s="40" customFormat="1">
       <c r="A97" s="49" t="s">
         <v>44</v>
       </c>
@@ -4430,7 +4429,7 @@
       </c>
       <c r="M97" s="44"/>
     </row>
-    <row r="98" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:15" s="40" customFormat="1">
       <c r="A98" s="49" t="s">
         <v>44</v>
       </c>
@@ -4457,7 +4456,7 @@
       </c>
       <c r="M98" s="44"/>
     </row>
-    <row r="99" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:15" s="40" customFormat="1">
       <c r="A99" s="49" t="s">
         <v>44</v>
       </c>
@@ -4484,7 +4483,7 @@
       </c>
       <c r="M99" s="44"/>
     </row>
-    <row r="100" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:15" s="40" customFormat="1">
       <c r="A100" s="49" t="s">
         <v>44</v>
       </c>
@@ -4511,7 +4510,7 @@
       </c>
       <c r="M100" s="44"/>
     </row>
-    <row r="101" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:15" s="40" customFormat="1">
       <c r="A101" s="49" t="s">
         <v>44</v>
       </c>
@@ -4538,7 +4537,7 @@
       </c>
       <c r="M101" s="44"/>
     </row>
-    <row r="102" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:15" s="40" customFormat="1">
       <c r="A102" s="49" t="s">
         <v>44</v>
       </c>
@@ -4565,7 +4564,7 @@
       </c>
       <c r="M102" s="44"/>
     </row>
-    <row r="103" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:15" s="40" customFormat="1">
       <c r="A103" s="49" t="s">
         <v>44</v>
       </c>
@@ -4592,7 +4591,7 @@
       </c>
       <c r="M103" s="44"/>
     </row>
-    <row r="104" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:15" s="40" customFormat="1">
       <c r="A104" s="49" t="s">
         <v>44</v>
       </c>
@@ -4619,7 +4618,7 @@
       </c>
       <c r="M104" s="44"/>
     </row>
-    <row r="105" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:15" s="40" customFormat="1">
       <c r="A105" s="49" t="s">
         <v>44</v>
       </c>
@@ -4646,7 +4645,7 @@
       </c>
       <c r="M105" s="44"/>
     </row>
-    <row r="106" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:15" s="40" customFormat="1">
       <c r="A106" s="49" t="s">
         <v>44</v>
       </c>
@@ -4673,7 +4672,7 @@
       </c>
       <c r="M106" s="44"/>
     </row>
-    <row r="107" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:15" s="40" customFormat="1">
       <c r="A107" s="49" t="s">
         <v>44</v>
       </c>
@@ -4700,7 +4699,7 @@
       </c>
       <c r="M107" s="44"/>
     </row>
-    <row r="108" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:15" s="40" customFormat="1">
       <c r="A108" s="49" t="s">
         <v>44</v>
       </c>
@@ -4727,7 +4726,7 @@
       </c>
       <c r="M108" s="44"/>
     </row>
-    <row r="109" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:15" s="40" customFormat="1">
       <c r="A109" s="49" t="s">
         <v>44</v>
       </c>
@@ -4754,7 +4753,7 @@
       </c>
       <c r="M109" s="44"/>
     </row>
-    <row r="110" spans="1:15" s="40" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:15" s="40" customFormat="1">
       <c r="A110" s="49" t="s">
         <v>44</v>
       </c>
@@ -4781,7 +4780,7 @@
       </c>
       <c r="M110" s="44"/>
     </row>
-    <row r="111" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:15" s="44" customFormat="1">
       <c r="A111" s="43"/>
       <c r="B111" s="43"/>
       <c r="C111" s="17"/>
@@ -4791,7 +4790,7 @@
       <c r="G111" s="41"/>
       <c r="H111" s="39"/>
     </row>
-    <row r="112" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:15">
       <c r="I112" s="19" t="s">
         <v>45</v>
       </c>
@@ -4808,7 +4807,7 @@
       <c r="N112" s="98"/>
       <c r="O112" s="123"/>
     </row>
-    <row r="113" spans="9:14" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="113" spans="9:14">
       <c r="I113" s="49" t="s">
         <v>45</v>
       </c>
@@ -4824,7 +4823,7 @@
       <c r="M113" s="44"/>
       <c r="N113" s="99"/>
     </row>
-    <row r="114" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="114" spans="9:14" s="44" customFormat="1">
       <c r="I114" s="49" t="s">
         <v>45</v>
       </c>
@@ -4839,7 +4838,7 @@
       </c>
       <c r="N114" s="96"/>
     </row>
-    <row r="115" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="115" spans="9:14" s="44" customFormat="1">
       <c r="I115" s="49" t="s">
         <v>45</v>
       </c>
@@ -4854,7 +4853,7 @@
       </c>
       <c r="N115" s="96"/>
     </row>
-    <row r="116" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="116" spans="9:14" s="44" customFormat="1">
       <c r="I116" s="49" t="s">
         <v>45</v>
       </c>
@@ -4869,7 +4868,7 @@
       </c>
       <c r="N116" s="96"/>
     </row>
-    <row r="117" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="117" spans="9:14" s="44" customFormat="1">
       <c r="I117" s="49" t="s">
         <v>45</v>
       </c>
@@ -4884,7 +4883,7 @@
       </c>
       <c r="N117" s="96"/>
     </row>
-    <row r="118" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="118" spans="9:14" s="44" customFormat="1">
       <c r="I118" s="49" t="s">
         <v>45</v>
       </c>
@@ -4899,7 +4898,7 @@
       </c>
       <c r="N118" s="100"/>
     </row>
-    <row r="119" spans="9:14" s="44" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="119" spans="9:14" s="44" customFormat="1">
       <c r="I119" s="49" t="s">
         <v>45</v>
       </c>
@@ -4914,7 +4913,7 @@
       </c>
       <c r="N119" s="96"/>
     </row>
-    <row r="120" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="9:14" s="44" customFormat="1">
       <c r="I120" s="49" t="s">
         <v>45</v>
       </c>
@@ -4929,7 +4928,7 @@
       </c>
       <c r="N120" s="97"/>
     </row>
-    <row r="121" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="9:14" s="44" customFormat="1">
       <c r="I121" s="49" t="s">
         <v>45</v>
       </c>
@@ -4944,7 +4943,7 @@
       </c>
       <c r="N121" s="97"/>
     </row>
-    <row r="122" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="9:14" s="44" customFormat="1">
       <c r="I122" s="49" t="s">
         <v>45</v>
       </c>
@@ -4959,7 +4958,7 @@
       </c>
       <c r="N122" s="97"/>
     </row>
-    <row r="123" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="9:14" s="44" customFormat="1">
       <c r="I123" s="49" t="s">
         <v>45</v>
       </c>
@@ -4974,7 +4973,7 @@
       </c>
       <c r="N123" s="97"/>
     </row>
-    <row r="124" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="9:14" s="44" customFormat="1">
       <c r="I124" s="49" t="s">
         <v>45</v>
       </c>
@@ -4989,7 +4988,7 @@
       </c>
       <c r="N124" s="97"/>
     </row>
-    <row r="125" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="9:14" s="44" customFormat="1">
       <c r="I125" s="49" t="s">
         <v>45</v>
       </c>
@@ -5004,7 +5003,7 @@
       </c>
       <c r="N125" s="97"/>
     </row>
-    <row r="126" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="9:14" s="44" customFormat="1">
       <c r="I126" s="49" t="s">
         <v>45</v>
       </c>
@@ -5019,7 +5018,7 @@
       </c>
       <c r="N126" s="97"/>
     </row>
-    <row r="127" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="9:14" s="44" customFormat="1">
       <c r="I127" s="49" t="s">
         <v>45</v>
       </c>
@@ -5034,7 +5033,7 @@
       </c>
       <c r="N127" s="97"/>
     </row>
-    <row r="128" spans="9:14" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="9:14" s="44" customFormat="1">
       <c r="I128" s="49" t="s">
         <v>45</v>
       </c>
@@ -5049,7 +5048,7 @@
       </c>
       <c r="N128" s="97"/>
     </row>
-    <row r="129" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:15" s="44" customFormat="1">
       <c r="I129" s="49" t="s">
         <v>45</v>
       </c>
@@ -5064,7 +5063,7 @@
       </c>
       <c r="N129" s="97"/>
     </row>
-    <row r="130" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:15" s="44" customFormat="1">
       <c r="I130" s="49" t="s">
         <v>45</v>
       </c>
@@ -5079,7 +5078,7 @@
       </c>
       <c r="N130" s="97"/>
     </row>
-    <row r="131" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:15" s="44" customFormat="1">
       <c r="I131" s="49" t="s">
         <v>45</v>
       </c>
@@ -5094,7 +5093,7 @@
       </c>
       <c r="N131" s="97"/>
     </row>
-    <row r="132" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:15" s="44" customFormat="1">
       <c r="I132" s="49" t="s">
         <v>45</v>
       </c>
@@ -5109,7 +5108,7 @@
       </c>
       <c r="N132" s="96"/>
     </row>
-    <row r="133" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:15" s="44" customFormat="1">
       <c r="I133" s="49" t="s">
         <v>45</v>
       </c>
@@ -5124,7 +5123,7 @@
       </c>
       <c r="N133" s="97"/>
     </row>
-    <row r="134" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:15" s="44" customFormat="1">
       <c r="I134" s="49" t="s">
         <v>45</v>
       </c>
@@ -5139,7 +5138,7 @@
       </c>
       <c r="N134" s="97"/>
     </row>
-    <row r="135" spans="1:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:15" s="44" customFormat="1">
       <c r="I135" s="49" t="s">
         <v>45</v>
       </c>
@@ -5154,7 +5153,7 @@
       </c>
       <c r="N135" s="97"/>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:15">
       <c r="A136" s="18"/>
       <c r="B136" s="42"/>
       <c r="C136" s="17"/>
@@ -5165,7 +5164,7 @@
       <c r="I136" s="1"/>
       <c r="M136" s="44"/>
     </row>
-    <row r="137" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:15">
       <c r="A137" s="16" t="s">
         <v>46</v>
       </c>
@@ -5193,7 +5192,7 @@
       <c r="I137" s="1"/>
       <c r="M137" s="44"/>
     </row>
-    <row r="138" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:15">
       <c r="A138" s="51" t="s">
         <v>46</v>
       </c>
@@ -5221,7 +5220,7 @@
       <c r="I138" s="1"/>
       <c r="M138" s="44"/>
     </row>
-    <row r="139" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:15">
       <c r="A139" s="51" t="s">
         <v>46</v>
       </c>
@@ -5249,7 +5248,7 @@
       <c r="I139" s="1"/>
       <c r="M139" s="44"/>
     </row>
-    <row r="140" spans="1:15" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:15" s="44" customFormat="1">
       <c r="A140" s="85" t="s">
         <v>46</v>
       </c>
@@ -5273,7 +5272,7 @@
       </c>
       <c r="H140" s="102"/>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:15">
       <c r="A141" s="18"/>
       <c r="B141" s="42"/>
       <c r="C141" s="17"/>
@@ -5284,7 +5283,7 @@
       <c r="I141" s="1"/>
       <c r="M141" s="44"/>
     </row>
-    <row r="142" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:15">
       <c r="I142" s="16" t="s">
         <v>47</v>
       </c>
@@ -5301,7 +5300,7 @@
       <c r="N142" s="103"/>
       <c r="O142" s="123"/>
     </row>
-    <row r="143" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:15">
       <c r="I143" s="51" t="s">
         <v>47</v>
       </c>
@@ -5317,7 +5316,7 @@
       <c r="M143" s="44"/>
       <c r="N143" s="103"/>
     </row>
-    <row r="144" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:15">
       <c r="I144" s="51" t="s">
         <v>47</v>
       </c>
@@ -5333,7 +5332,7 @@
       <c r="M144" s="44"/>
       <c r="N144" s="104"/>
     </row>
-    <row r="145" spans="1:22" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:22" s="44" customFormat="1">
       <c r="I145" s="85" t="s">
         <v>47</v>
       </c>
@@ -5348,7 +5347,7 @@
       </c>
       <c r="N145" s="105"/>
     </row>
-    <row r="146" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:22">
       <c r="I146" s="18"/>
       <c r="J146" s="17"/>
       <c r="K146" s="45"/>
@@ -5356,7 +5355,7 @@
       <c r="M146" s="44"/>
       <c r="N146" s="29"/>
     </row>
-    <row r="147" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:22">
       <c r="A147" s="119" t="s">
         <v>136</v>
       </c>
@@ -5386,7 +5385,7 @@
       </c>
       <c r="M147" s="44"/>
     </row>
-    <row r="148" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:22">
       <c r="A148" s="50" t="s">
         <v>136</v>
       </c>
@@ -5416,7 +5415,7 @@
       </c>
       <c r="M148" s="44"/>
     </row>
-    <row r="149" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:22">
       <c r="A149" s="50" t="s">
         <v>136</v>
       </c>
@@ -5444,7 +5443,7 @@
       <c r="I149" s="1"/>
       <c r="M149" s="44"/>
     </row>
-    <row r="150" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:22">
       <c r="A150" s="50" t="s">
         <v>136</v>
       </c>
@@ -5472,7 +5471,7 @@
       <c r="I150" s="1"/>
       <c r="M150" s="44"/>
     </row>
-    <row r="151" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:22">
       <c r="A151" s="50" t="s">
         <v>136</v>
       </c>
@@ -5500,7 +5499,7 @@
       <c r="I151" s="1"/>
       <c r="M151" s="44"/>
     </row>
-    <row r="152" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:22">
       <c r="A152" s="50" t="s">
         <v>136</v>
       </c>
@@ -5528,7 +5527,7 @@
       <c r="I152" s="1"/>
       <c r="M152" s="44"/>
     </row>
-    <row r="153" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:22">
       <c r="A153" s="50" t="s">
         <v>136</v>
       </c>
@@ -5556,7 +5555,7 @@
       <c r="I153" s="1"/>
       <c r="M153" s="44"/>
     </row>
-    <row r="154" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:22">
       <c r="A154" s="18"/>
       <c r="B154" s="42"/>
       <c r="C154" s="17"/>
@@ -5567,7 +5566,7 @@
       <c r="I154" s="1"/>
       <c r="M154" s="44"/>
     </row>
-    <row r="155" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:22">
       <c r="A155" s="33" t="s">
         <v>137</v>
       </c>
@@ -5599,7 +5598,7 @@
       <c r="U155" s="40"/>
       <c r="V155" s="40"/>
     </row>
-    <row r="156" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:22">
       <c r="A156" s="52" t="s">
         <v>137</v>
       </c>
@@ -5631,7 +5630,7 @@
       <c r="U156" s="40"/>
       <c r="V156" s="40"/>
     </row>
-    <row r="157" spans="1:22" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:22">
       <c r="A157" s="52" t="s">
         <v>137</v>
       </c>
@@ -5659,7 +5658,7 @@
       <c r="I157" s="1"/>
       <c r="M157" s="44"/>
     </row>
-    <row r="158" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:22">
       <c r="A158" s="18"/>
       <c r="B158" s="42"/>
       <c r="C158" s="17"/>
@@ -5670,7 +5669,7 @@
       <c r="I158" s="1"/>
       <c r="M158" s="44"/>
     </row>
-    <row r="159" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:22">
       <c r="I159" s="34" t="s">
         <v>58</v>
       </c>
@@ -5687,7 +5686,7 @@
       <c r="N159" s="107"/>
       <c r="O159" s="123"/>
     </row>
-    <row r="160" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:22">
       <c r="I160" s="52" t="s">
         <v>58</v>
       </c>
@@ -5703,7 +5702,7 @@
       <c r="M160" s="44"/>
       <c r="N160" s="98"/>
     </row>
-    <row r="161" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="161" spans="9:22">
       <c r="I161" s="52" t="s">
         <v>58</v>
       </c>
@@ -5719,7 +5718,7 @@
       <c r="M161" s="44"/>
       <c r="N161" s="99"/>
     </row>
-    <row r="162" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="162" spans="9:22">
       <c r="I162" s="52" t="s">
         <v>58</v>
       </c>
@@ -5738,7 +5737,7 @@
       <c r="U162" s="44"/>
       <c r="V162" s="44"/>
     </row>
-    <row r="163" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="163" spans="9:22">
       <c r="I163" s="52" t="s">
         <v>58</v>
       </c>
@@ -5754,7 +5753,7 @@
       <c r="M163" s="44"/>
       <c r="N163" s="107"/>
     </row>
-    <row r="164" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="164" spans="9:22">
       <c r="I164" s="52" t="s">
         <v>58</v>
       </c>
@@ -5770,7 +5769,7 @@
       <c r="M164" s="44"/>
       <c r="N164" s="107"/>
     </row>
-    <row r="165" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="165" spans="9:22">
       <c r="I165" s="52" t="s">
         <v>58</v>
       </c>
@@ -5786,7 +5785,7 @@
       <c r="M165" s="44"/>
       <c r="N165" s="107"/>
     </row>
-    <row r="166" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="166" spans="9:22">
       <c r="I166" s="18"/>
       <c r="J166" s="17"/>
       <c r="K166" s="45"/>
@@ -5794,7 +5793,7 @@
       <c r="M166" s="44"/>
       <c r="N166" s="18"/>
     </row>
-    <row r="167" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="167" spans="9:22">
       <c r="I167" s="34" t="s">
         <v>59</v>
       </c>
@@ -5811,7 +5810,7 @@
       <c r="N167" s="108"/>
       <c r="O167" s="123"/>
     </row>
-    <row r="168" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="168" spans="9:22">
       <c r="I168" s="52" t="s">
         <v>59</v>
       </c>
@@ -5827,7 +5826,7 @@
       <c r="M168" s="44"/>
       <c r="N168" s="108"/>
     </row>
-    <row r="169" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="169" spans="9:22">
       <c r="I169" s="52" t="s">
         <v>59</v>
       </c>
@@ -5843,7 +5842,7 @@
       <c r="M169" s="44"/>
       <c r="N169" s="108"/>
     </row>
-    <row r="170" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="170" spans="9:22">
       <c r="I170" s="52" t="s">
         <v>59</v>
       </c>
@@ -5859,7 +5858,7 @@
       <c r="M170" s="44"/>
       <c r="N170" s="108"/>
     </row>
-    <row r="171" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="171" spans="9:22">
       <c r="I171" s="52" t="s">
         <v>59</v>
       </c>
@@ -5875,7 +5874,7 @@
       <c r="M171" s="44"/>
       <c r="N171" s="108"/>
     </row>
-    <row r="172" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="172" spans="9:22">
       <c r="I172" s="52" t="s">
         <v>59</v>
       </c>
@@ -5891,7 +5890,7 @@
       <c r="M172" s="44"/>
       <c r="N172" s="71"/>
     </row>
-    <row r="173" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="173" spans="9:22">
       <c r="I173" s="52" t="s">
         <v>59</v>
       </c>
@@ -5907,7 +5906,7 @@
       <c r="M173" s="44"/>
       <c r="N173" s="108"/>
     </row>
-    <row r="174" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="174" spans="9:22">
       <c r="I174" s="52" t="s">
         <v>59</v>
       </c>
@@ -5923,7 +5922,7 @@
       <c r="M174" s="44"/>
       <c r="N174" s="71"/>
     </row>
-    <row r="175" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="175" spans="9:22">
       <c r="I175" s="52" t="s">
         <v>59</v>
       </c>
@@ -5939,7 +5938,7 @@
       <c r="M175" s="44"/>
       <c r="N175" s="108"/>
     </row>
-    <row r="176" spans="9:22" x14ac:dyDescent="0.2">
+    <row r="176" spans="9:22">
       <c r="I176" s="52" t="s">
         <v>59</v>
       </c>
@@ -5955,7 +5954,7 @@
       <c r="M176" s="44"/>
       <c r="N176" s="108"/>
     </row>
-    <row r="177" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="177" spans="9:15">
       <c r="I177" s="52" t="s">
         <v>59</v>
       </c>
@@ -5971,7 +5970,7 @@
       <c r="M177" s="44"/>
       <c r="N177" s="108"/>
     </row>
-    <row r="178" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="178" spans="9:15">
       <c r="I178" s="52" t="s">
         <v>59</v>
       </c>
@@ -5987,7 +5986,7 @@
       <c r="M178" s="44"/>
       <c r="N178" s="108"/>
     </row>
-    <row r="179" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="179" spans="9:15">
       <c r="I179" s="52" t="s">
         <v>59</v>
       </c>
@@ -6003,7 +6002,7 @@
       <c r="M179" s="44"/>
       <c r="N179" s="108"/>
     </row>
-    <row r="180" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="180" spans="9:15">
       <c r="I180" s="52" t="s">
         <v>59</v>
       </c>
@@ -6019,7 +6018,7 @@
       <c r="M180" s="44"/>
       <c r="N180" s="108"/>
     </row>
-    <row r="181" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="181" spans="9:15">
       <c r="I181" s="52" t="s">
         <v>59</v>
       </c>
@@ -6035,7 +6034,7 @@
       <c r="M181" s="44"/>
       <c r="N181" s="108"/>
     </row>
-    <row r="182" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="182" spans="9:15">
       <c r="I182" s="52" t="s">
         <v>59</v>
       </c>
@@ -6051,7 +6050,7 @@
       <c r="M182" s="44"/>
       <c r="N182" s="109"/>
     </row>
-    <row r="183" spans="9:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="9:15" s="44" customFormat="1">
       <c r="I183" s="52" t="s">
         <v>59</v>
       </c>
@@ -6066,7 +6065,7 @@
       </c>
       <c r="N183" s="110"/>
     </row>
-    <row r="184" spans="9:15" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="9:15" s="44" customFormat="1">
       <c r="I184" s="52" t="s">
         <v>59</v>
       </c>
@@ -6081,7 +6080,7 @@
       </c>
       <c r="N184" s="110"/>
     </row>
-    <row r="185" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="185" spans="9:15">
       <c r="I185" s="18"/>
       <c r="J185" s="17"/>
       <c r="K185" s="45"/>
@@ -6089,7 +6088,7 @@
       <c r="M185" s="44"/>
       <c r="N185" s="18"/>
     </row>
-    <row r="186" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="186" spans="9:15">
       <c r="I186" s="34" t="s">
         <v>60</v>
       </c>
@@ -6106,7 +6105,7 @@
       <c r="N186" s="111"/>
       <c r="O186" s="123"/>
     </row>
-    <row r="187" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="187" spans="9:15">
       <c r="I187" s="52" t="s">
         <v>60</v>
       </c>
@@ -6122,7 +6121,7 @@
       <c r="M187" s="44"/>
       <c r="N187" s="111"/>
     </row>
-    <row r="188" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="188" spans="9:15">
       <c r="I188" s="52" t="s">
         <v>60</v>
       </c>
@@ -6138,7 +6137,7 @@
       <c r="M188" s="44"/>
       <c r="N188" s="111"/>
     </row>
-    <row r="189" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="189" spans="9:15">
       <c r="I189" s="52" t="s">
         <v>60</v>
       </c>
@@ -6154,7 +6153,7 @@
       <c r="M189" s="44"/>
       <c r="N189" s="111"/>
     </row>
-    <row r="190" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="190" spans="9:15">
       <c r="I190" s="52" t="s">
         <v>60</v>
       </c>
@@ -6170,7 +6169,7 @@
       <c r="M190" s="44"/>
       <c r="N190" s="94"/>
     </row>
-    <row r="191" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="191" spans="9:15">
       <c r="I191" s="52" t="s">
         <v>60</v>
       </c>
@@ -6186,7 +6185,7 @@
       <c r="M191" s="44"/>
       <c r="N191" s="94"/>
     </row>
-    <row r="192" spans="9:15" x14ac:dyDescent="0.2">
+    <row r="192" spans="9:15">
       <c r="I192" s="52" t="s">
         <v>60</v>
       </c>
@@ -6202,7 +6201,7 @@
       <c r="M192" s="44"/>
       <c r="N192" s="94"/>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:17">
       <c r="I193" s="52" t="s">
         <v>60</v>
       </c>
@@ -6218,7 +6217,7 @@
       <c r="M193" s="44"/>
       <c r="N193" s="94"/>
     </row>
-    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:17">
       <c r="A194" s="23"/>
       <c r="B194" s="23"/>
       <c r="C194" s="46"/>
@@ -6227,7 +6226,7 @@
       <c r="I194" s="1"/>
       <c r="M194" s="44"/>
     </row>
-    <row r="195" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:17" s="44" customFormat="1">
       <c r="I195" s="79" t="s">
         <v>110</v>
       </c>
@@ -6243,7 +6242,7 @@
       <c r="N195" s="76"/>
       <c r="O195" s="123"/>
     </row>
-    <row r="196" spans="1:17" s="44" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" s="44" customFormat="1">
       <c r="A196" s="82"/>
       <c r="B196" s="82"/>
       <c r="C196" s="83"/>
@@ -6257,7 +6256,7 @@
       <c r="N196" s="73"/>
       <c r="O196" s="73"/>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:17">
       <c r="I197" s="78" t="s">
         <v>109</v>
       </c>
@@ -6276,7 +6275,7 @@
       <c r="P197" s="44"/>
       <c r="Q197" s="44"/>
     </row>
-    <row r="198" spans="1:17" s="44" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:17" s="44" customFormat="1">
       <c r="A198" s="23"/>
       <c r="B198" s="23"/>
       <c r="C198" s="17"/>
@@ -6286,7 +6285,7 @@
       <c r="H198" s="45"/>
       <c r="I198" s="72"/>
     </row>
-    <row r="199" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17">
       <c r="A199" s="19" t="s">
         <v>85</v>
       </c>
@@ -6310,7 +6309,7 @@
       <c r="I199" s="1"/>
       <c r="M199" s="44"/>
     </row>
-    <row r="200" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17">
       <c r="I200" s="18" t="s">
         <v>83</v>
       </c>
@@ -6326,7 +6325,7 @@
       <c r="M200" s="44"/>
       <c r="N200" s="35"/>
     </row>
-    <row r="201" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17">
       <c r="I201" s="18" t="s">
         <v>84</v>
       </c>
@@ -6343,7 +6342,7 @@
       <c r="N201" s="35"/>
       <c r="O201" s="123"/>
     </row>
-    <row r="202" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17">
       <c r="A202" s="18"/>
       <c r="B202" s="42"/>
       <c r="C202" s="17"/>
@@ -6354,7 +6353,7 @@
       <c r="I202" s="1"/>
       <c r="M202" s="44"/>
     </row>
-    <row r="203" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:17">
       <c r="A203" s="19" t="s">
         <v>91</v>
       </c>
@@ -6379,7 +6378,7 @@
       <c r="J203" s="44"/>
       <c r="M203" s="44"/>
     </row>
-    <row r="204" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17">
       <c r="A204" s="18" t="s">
         <v>86</v>
       </c>
@@ -6404,7 +6403,7 @@
       <c r="J204" s="44"/>
       <c r="M204" s="44"/>
     </row>
-    <row r="205" spans="1:17" ht="15" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17">
       <c r="A205" s="18" t="s">
         <v>87</v>
       </c>
@@ -6429,7 +6428,7 @@
       <c r="J205" s="44"/>
       <c r="M205" s="44"/>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:17">
       <c r="I206" s="18" t="s">
         <v>88</v>
       </c>
@@ -6446,7 +6445,7 @@
       <c r="N206" s="44"/>
       <c r="O206" s="73"/>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:17">
       <c r="I207" s="18" t="s">
         <v>89</v>
       </c>
@@ -6463,7 +6462,7 @@
       <c r="N207" s="44"/>
       <c r="O207" s="123"/>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:17">
       <c r="I208" s="18" t="s">
         <v>90</v>
       </c>
@@ -6480,633 +6479,633 @@
       <c r="N208" s="44"/>
       <c r="O208" s="123"/>
     </row>
-    <row r="209" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="209" spans="9:13">
       <c r="I209" s="1"/>
       <c r="M209" s="44"/>
     </row>
-    <row r="210" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="210" spans="9:13">
       <c r="I210" s="1"/>
       <c r="M210" s="44"/>
     </row>
-    <row r="211" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="211" spans="9:13">
       <c r="I211" s="1"/>
       <c r="M211" s="44"/>
     </row>
-    <row r="212" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="212" spans="9:13">
       <c r="I212" s="1"/>
       <c r="M212" s="44"/>
     </row>
-    <row r="213" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="213" spans="9:13">
       <c r="I213" s="1"/>
       <c r="M213" s="44"/>
     </row>
-    <row r="214" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="214" spans="9:13">
       <c r="I214" s="1"/>
       <c r="M214" s="44"/>
     </row>
-    <row r="215" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="215" spans="9:13">
       <c r="I215" s="1"/>
       <c r="M215" s="44"/>
     </row>
-    <row r="216" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="216" spans="9:13">
       <c r="I216" s="1"/>
       <c r="M216" s="44"/>
     </row>
-    <row r="217" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="217" spans="9:13">
       <c r="I217" s="1"/>
       <c r="M217" s="44"/>
     </row>
-    <row r="218" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="218" spans="9:13">
       <c r="I218" s="1"/>
       <c r="M218" s="44"/>
     </row>
-    <row r="219" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="219" spans="9:13">
       <c r="I219" s="1"/>
       <c r="M219" s="44"/>
     </row>
-    <row r="220" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="220" spans="9:13">
       <c r="I220" s="1"/>
       <c r="M220" s="44"/>
     </row>
-    <row r="221" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="221" spans="9:13">
       <c r="I221" s="1"/>
       <c r="M221" s="44"/>
     </row>
-    <row r="222" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="222" spans="9:13">
       <c r="I222" s="1"/>
       <c r="M222" s="44"/>
     </row>
-    <row r="223" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="223" spans="9:13">
       <c r="I223" s="1"/>
       <c r="M223" s="44"/>
     </row>
-    <row r="224" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="224" spans="9:13">
       <c r="I224" s="1"/>
       <c r="M224" s="44"/>
     </row>
-    <row r="225" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="225" spans="9:13">
       <c r="I225" s="1"/>
       <c r="M225" s="44"/>
     </row>
-    <row r="226" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="226" spans="9:13">
       <c r="I226" s="1"/>
       <c r="M226" s="44"/>
     </row>
-    <row r="227" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="227" spans="9:13">
       <c r="I227" s="1"/>
       <c r="M227" s="44"/>
     </row>
-    <row r="228" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="228" spans="9:13">
       <c r="I228" s="1"/>
       <c r="M228" s="44"/>
     </row>
-    <row r="229" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="229" spans="9:13">
       <c r="I229" s="1"/>
       <c r="M229" s="44"/>
     </row>
-    <row r="230" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="230" spans="9:13">
       <c r="I230" s="1"/>
       <c r="M230" s="44"/>
     </row>
-    <row r="231" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="231" spans="9:13">
       <c r="I231" s="1"/>
       <c r="M231" s="44"/>
     </row>
-    <row r="232" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="232" spans="9:13">
       <c r="I232" s="1"/>
       <c r="M232" s="44"/>
     </row>
-    <row r="233" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="233" spans="9:13">
       <c r="I233" s="1"/>
       <c r="M233" s="44"/>
     </row>
-    <row r="234" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="234" spans="9:13">
       <c r="I234" s="1"/>
       <c r="M234" s="44"/>
     </row>
-    <row r="235" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="235" spans="9:13">
       <c r="I235" s="1"/>
       <c r="M235" s="44"/>
     </row>
-    <row r="236" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="236" spans="9:13">
       <c r="I236" s="1"/>
       <c r="M236" s="44"/>
     </row>
-    <row r="237" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="237" spans="9:13">
       <c r="I237" s="1"/>
       <c r="M237" s="44"/>
     </row>
-    <row r="238" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="238" spans="9:13">
       <c r="I238" s="1"/>
       <c r="M238" s="44"/>
     </row>
-    <row r="239" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="239" spans="9:13">
       <c r="I239" s="1"/>
       <c r="M239" s="44"/>
     </row>
-    <row r="240" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="240" spans="9:13">
       <c r="I240" s="1"/>
       <c r="M240" s="44"/>
     </row>
-    <row r="241" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="241" spans="9:13">
       <c r="I241" s="1"/>
       <c r="M241" s="44"/>
     </row>
-    <row r="242" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="242" spans="9:13">
       <c r="I242" s="1"/>
       <c r="M242" s="44"/>
     </row>
-    <row r="243" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="243" spans="9:13">
       <c r="I243" s="1"/>
       <c r="M243" s="44"/>
     </row>
-    <row r="244" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="244" spans="9:13">
       <c r="I244" s="1"/>
       <c r="M244" s="44"/>
     </row>
-    <row r="245" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="245" spans="9:13">
       <c r="I245" s="1"/>
       <c r="M245" s="44"/>
     </row>
-    <row r="246" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="246" spans="9:13">
       <c r="I246" s="1"/>
       <c r="M246" s="44"/>
     </row>
-    <row r="247" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="247" spans="9:13">
       <c r="I247" s="1"/>
       <c r="M247" s="44"/>
     </row>
-    <row r="248" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="248" spans="9:13">
       <c r="I248" s="1"/>
       <c r="M248" s="44"/>
     </row>
-    <row r="249" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="249" spans="9:13">
       <c r="I249" s="1"/>
       <c r="M249" s="44"/>
     </row>
-    <row r="250" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="250" spans="9:13">
       <c r="I250" s="1"/>
       <c r="M250" s="44"/>
     </row>
-    <row r="251" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="251" spans="9:13">
       <c r="I251" s="1"/>
       <c r="M251" s="44"/>
     </row>
-    <row r="252" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="252" spans="9:13">
       <c r="I252" s="1"/>
       <c r="M252" s="44"/>
     </row>
-    <row r="253" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="253" spans="9:13">
       <c r="I253" s="1"/>
       <c r="M253" s="44"/>
     </row>
-    <row r="254" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="254" spans="9:13">
       <c r="I254" s="1"/>
       <c r="M254" s="44"/>
     </row>
-    <row r="255" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="255" spans="9:13">
       <c r="I255" s="1"/>
       <c r="M255" s="44"/>
     </row>
-    <row r="256" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="256" spans="9:13">
       <c r="I256" s="1"/>
       <c r="M256" s="44"/>
     </row>
-    <row r="257" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="257" spans="9:13">
       <c r="I257" s="1"/>
       <c r="M257" s="44"/>
     </row>
-    <row r="258" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="258" spans="9:13">
       <c r="I258" s="1"/>
       <c r="M258" s="44"/>
     </row>
-    <row r="259" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="259" spans="9:13">
       <c r="I259" s="1"/>
       <c r="M259" s="44"/>
     </row>
-    <row r="260" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="9:13">
       <c r="I260" s="1"/>
       <c r="M260" s="44"/>
     </row>
-    <row r="261" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="9:13">
       <c r="I261" s="1"/>
       <c r="M261" s="44"/>
     </row>
-    <row r="262" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="262" spans="9:13">
       <c r="I262" s="1"/>
       <c r="M262" s="44"/>
     </row>
-    <row r="263" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="263" spans="9:13">
       <c r="I263" s="1"/>
       <c r="M263" s="44"/>
     </row>
-    <row r="264" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="264" spans="9:13">
       <c r="I264" s="1"/>
       <c r="M264" s="44"/>
     </row>
-    <row r="265" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="9:13">
       <c r="I265" s="1"/>
       <c r="M265" s="44"/>
     </row>
-    <row r="266" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="266" spans="9:13">
       <c r="I266" s="1"/>
       <c r="M266" s="44"/>
     </row>
-    <row r="267" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="9:13">
       <c r="I267" s="1"/>
       <c r="M267" s="44"/>
     </row>
-    <row r="268" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="268" spans="9:13">
       <c r="I268" s="1"/>
       <c r="M268" s="44"/>
     </row>
-    <row r="269" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="269" spans="9:13">
       <c r="I269" s="1"/>
       <c r="M269" s="44"/>
     </row>
-    <row r="270" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="9:13">
       <c r="I270" s="1"/>
       <c r="M270" s="44"/>
     </row>
-    <row r="271" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="271" spans="9:13">
       <c r="I271" s="1"/>
       <c r="M271" s="44"/>
     </row>
-    <row r="272" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="272" spans="9:13">
       <c r="I272" s="1"/>
       <c r="M272" s="44"/>
     </row>
-    <row r="273" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="273" spans="9:13">
       <c r="I273" s="1"/>
       <c r="M273" s="44"/>
     </row>
-    <row r="274" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="274" spans="9:13">
       <c r="I274" s="1"/>
       <c r="M274" s="44"/>
     </row>
-    <row r="275" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="275" spans="9:13">
       <c r="I275" s="1"/>
       <c r="M275" s="44"/>
     </row>
-    <row r="276" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="276" spans="9:13">
       <c r="I276" s="1"/>
       <c r="M276" s="44"/>
     </row>
-    <row r="277" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="277" spans="9:13">
       <c r="I277" s="1"/>
       <c r="M277" s="44"/>
     </row>
-    <row r="278" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="278" spans="9:13">
       <c r="I278" s="1"/>
       <c r="M278" s="44"/>
     </row>
-    <row r="279" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="279" spans="9:13">
       <c r="I279" s="1"/>
       <c r="M279" s="44"/>
     </row>
-    <row r="280" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="280" spans="9:13">
       <c r="I280" s="1"/>
       <c r="M280" s="44"/>
     </row>
-    <row r="281" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="281" spans="9:13">
       <c r="I281" s="1"/>
       <c r="M281" s="44"/>
     </row>
-    <row r="282" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="282" spans="9:13">
       <c r="I282" s="1"/>
       <c r="M282" s="44"/>
     </row>
-    <row r="283" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="283" spans="9:13">
       <c r="I283" s="1"/>
       <c r="M283" s="44"/>
     </row>
-    <row r="284" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="284" spans="9:13">
       <c r="I284" s="1"/>
       <c r="M284" s="44"/>
     </row>
-    <row r="285" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="285" spans="9:13">
       <c r="I285" s="1"/>
       <c r="M285" s="44"/>
     </row>
-    <row r="286" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="286" spans="9:13">
       <c r="I286" s="1"/>
       <c r="M286" s="44"/>
     </row>
-    <row r="287" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="287" spans="9:13">
       <c r="I287" s="1"/>
       <c r="M287" s="44"/>
     </row>
-    <row r="288" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="288" spans="9:13">
       <c r="I288" s="1"/>
       <c r="M288" s="44"/>
     </row>
-    <row r="289" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="9:13">
       <c r="I289" s="1"/>
       <c r="M289" s="44"/>
     </row>
-    <row r="290" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="9:13">
       <c r="I290" s="1"/>
       <c r="M290" s="44"/>
     </row>
-    <row r="291" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="9:13">
       <c r="I291" s="1"/>
       <c r="M291" s="44"/>
     </row>
-    <row r="292" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="9:13">
       <c r="I292" s="1"/>
       <c r="M292" s="44"/>
     </row>
-    <row r="293" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="9:13">
       <c r="I293" s="1"/>
       <c r="M293" s="44"/>
     </row>
-    <row r="294" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="9:13">
       <c r="I294" s="1"/>
       <c r="M294" s="44"/>
     </row>
-    <row r="295" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="295" spans="9:13">
       <c r="I295" s="1"/>
       <c r="M295" s="44"/>
     </row>
-    <row r="296" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="9:13">
       <c r="I296" s="1"/>
       <c r="M296" s="44"/>
     </row>
-    <row r="297" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="9:13">
       <c r="I297" s="1"/>
       <c r="M297" s="44"/>
     </row>
-    <row r="298" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="9:13">
       <c r="I298" s="1"/>
       <c r="M298" s="44"/>
     </row>
-    <row r="299" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="9:13">
       <c r="I299" s="1"/>
       <c r="M299" s="44"/>
     </row>
-    <row r="300" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="9:13">
       <c r="I300" s="1"/>
       <c r="M300" s="44"/>
     </row>
-    <row r="301" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="9:13">
       <c r="I301" s="1"/>
       <c r="M301" s="44"/>
     </row>
-    <row r="302" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="9:13">
       <c r="I302" s="1"/>
       <c r="M302" s="44"/>
     </row>
-    <row r="303" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="9:13">
       <c r="I303" s="1"/>
       <c r="M303" s="44"/>
     </row>
-    <row r="304" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="304" spans="9:13">
       <c r="I304" s="1"/>
       <c r="M304" s="44"/>
     </row>
-    <row r="305" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="305" spans="9:13">
       <c r="I305" s="1"/>
       <c r="M305" s="44"/>
     </row>
-    <row r="306" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="306" spans="9:13">
       <c r="I306" s="1"/>
       <c r="M306" s="44"/>
     </row>
-    <row r="307" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="307" spans="9:13">
       <c r="I307" s="1"/>
       <c r="M307" s="44"/>
     </row>
-    <row r="308" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="308" spans="9:13">
       <c r="I308" s="1"/>
       <c r="M308" s="44"/>
     </row>
-    <row r="309" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="309" spans="9:13">
       <c r="I309" s="1"/>
       <c r="M309" s="44"/>
     </row>
-    <row r="310" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="310" spans="9:13">
       <c r="I310" s="1"/>
       <c r="M310" s="44"/>
     </row>
-    <row r="311" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="311" spans="9:13">
       <c r="I311" s="1"/>
       <c r="M311" s="44"/>
     </row>
-    <row r="312" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="312" spans="9:13">
       <c r="I312" s="1"/>
       <c r="M312" s="44"/>
     </row>
-    <row r="313" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="313" spans="9:13">
       <c r="I313" s="1"/>
     </row>
-    <row r="314" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="314" spans="9:13">
       <c r="I314" s="1"/>
     </row>
-    <row r="315" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="315" spans="9:13">
       <c r="I315" s="1"/>
     </row>
-    <row r="316" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="316" spans="9:13">
       <c r="I316" s="1"/>
     </row>
-    <row r="317" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="317" spans="9:13">
       <c r="I317" s="1"/>
     </row>
-    <row r="318" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="318" spans="9:13">
       <c r="I318" s="1"/>
     </row>
-    <row r="319" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="319" spans="9:13">
       <c r="I319" s="1"/>
     </row>
-    <row r="320" spans="9:13" x14ac:dyDescent="0.25">
+    <row r="320" spans="9:13">
       <c r="I320" s="1"/>
     </row>
-    <row r="321" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="9:9">
       <c r="I321" s="1"/>
     </row>
-    <row r="322" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="9:9">
       <c r="I322" s="1"/>
     </row>
-    <row r="323" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="9:9">
       <c r="I323" s="1"/>
     </row>
-    <row r="324" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="9:9">
       <c r="I324" s="1"/>
     </row>
-    <row r="325" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="9:9">
       <c r="I325" s="1"/>
     </row>
-    <row r="326" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="9:9">
       <c r="I326" s="1"/>
     </row>
-    <row r="327" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="9:9">
       <c r="I327" s="1"/>
     </row>
-    <row r="328" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="9:9">
       <c r="I328" s="1"/>
     </row>
-    <row r="329" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="9:9">
       <c r="I329" s="1"/>
     </row>
-    <row r="330" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="9:9">
       <c r="I330" s="1"/>
     </row>
-    <row r="331" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="9:9">
       <c r="I331" s="1"/>
     </row>
-    <row r="332" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="9:9">
       <c r="I332" s="1"/>
     </row>
-    <row r="333" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="9:9">
       <c r="I333" s="1"/>
     </row>
-    <row r="334" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="9:9">
       <c r="I334" s="1"/>
     </row>
-    <row r="335" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="9:9">
       <c r="I335" s="1"/>
     </row>
-    <row r="336" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="9:9">
       <c r="I336" s="1"/>
     </row>
-    <row r="337" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="9:9">
       <c r="I337" s="1"/>
     </row>
-    <row r="338" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="9:9">
       <c r="I338" s="1"/>
     </row>
-    <row r="339" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="9:9">
       <c r="I339" s="1"/>
     </row>
-    <row r="340" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="9:9">
       <c r="I340" s="1"/>
     </row>
-    <row r="341" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="341" spans="9:9">
       <c r="I341" s="1"/>
     </row>
-    <row r="342" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="9:9">
       <c r="I342" s="1"/>
     </row>
-    <row r="343" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="9:9">
       <c r="I343" s="1"/>
     </row>
-    <row r="344" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="9:9">
       <c r="I344" s="1"/>
     </row>
-    <row r="345" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="9:9">
       <c r="I345" s="1"/>
     </row>
-    <row r="346" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="9:9">
       <c r="I346" s="1"/>
     </row>
-    <row r="347" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="9:9">
       <c r="I347" s="1"/>
     </row>
-    <row r="348" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="9:9">
       <c r="I348" s="1"/>
     </row>
-    <row r="349" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="9:9">
       <c r="I349" s="1"/>
     </row>
-    <row r="350" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="9:9">
       <c r="I350" s="1"/>
     </row>
-    <row r="351" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="9:9">
       <c r="I351" s="1"/>
     </row>
-    <row r="352" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="9:9">
       <c r="I352" s="1"/>
     </row>
-    <row r="353" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="353" spans="9:9">
       <c r="I353" s="1"/>
     </row>
-    <row r="354" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="354" spans="9:9">
       <c r="I354" s="1"/>
     </row>
-    <row r="355" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="355" spans="9:9">
       <c r="I355" s="1"/>
     </row>
-    <row r="356" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="356" spans="9:9">
       <c r="I356" s="1"/>
     </row>
-    <row r="357" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="9:9">
       <c r="I357" s="1"/>
     </row>
-    <row r="358" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="358" spans="9:9">
       <c r="I358" s="1"/>
     </row>
-    <row r="359" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="359" spans="9:9">
       <c r="I359" s="1"/>
     </row>
-    <row r="360" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="360" spans="9:9">
       <c r="I360" s="1"/>
     </row>
-    <row r="361" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="361" spans="9:9">
       <c r="I361" s="1"/>
     </row>
-    <row r="362" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="9:9">
       <c r="I362" s="1"/>
     </row>
-    <row r="363" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="363" spans="9:9">
       <c r="I363" s="1"/>
     </row>
-    <row r="364" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="364" spans="9:9">
       <c r="I364" s="1"/>
     </row>
-    <row r="365" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="365" spans="9:9">
       <c r="I365" s="1"/>
     </row>
-    <row r="366" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="366" spans="9:9">
       <c r="I366" s="1"/>
     </row>
-    <row r="367" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="367" spans="9:9">
       <c r="I367" s="1"/>
     </row>
-    <row r="368" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="368" spans="9:9">
       <c r="I368" s="1"/>
     </row>
-    <row r="369" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="369" spans="9:9">
       <c r="I369" s="1"/>
     </row>
-    <row r="370" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="9:9">
       <c r="I370" s="1"/>
     </row>
-    <row r="371" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="9:9">
       <c r="I371" s="1"/>
     </row>
-    <row r="372" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="9:9">
       <c r="I372" s="1"/>
     </row>
-    <row r="373" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="9:9">
       <c r="I373" s="1"/>
     </row>
-    <row r="374" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="9:9">
       <c r="I374" s="1"/>
     </row>
-    <row r="375" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="375" spans="9:9">
       <c r="I375" s="1"/>
     </row>
-    <row r="376" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="9:9">
       <c r="I376" s="1"/>
     </row>
-    <row r="377" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="9:9">
       <c r="I377" s="1"/>
     </row>
-    <row r="378" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="9:9">
       <c r="I378" s="1"/>
     </row>
-    <row r="379" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="9:9">
       <c r="I379" s="1"/>
     </row>
-    <row r="380" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="9:9">
       <c r="I380" s="1"/>
     </row>
-    <row r="381" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="9:9">
       <c r="I381" s="1"/>
     </row>
-    <row r="382" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="382" spans="9:9">
       <c r="I382" s="1"/>
     </row>
-    <row r="383" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="383" spans="9:9">
       <c r="I383" s="1"/>
     </row>
   </sheetData>
@@ -7128,12 +7127,12 @@
       <selection activeCell="R69" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="112"/>
+    <col min="1" max="16384" width="8.83203125" style="112"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="A1" s="112">
         <v>-0.102899</v>
       </c>
@@ -7246,7 +7245,7 @@
         <v>4.7835000000000003E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" s="112">
         <v>-9.2008999999999994E-2</v>
       </c>
@@ -7359,7 +7358,7 @@
         <v>3.9530999999999997E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="112">
         <v>-7.9813999999999996E-2</v>
       </c>
@@ -7472,7 +7471,7 @@
         <v>3.2724000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="112">
         <v>-6.7954000000000001E-2</v>
       </c>
@@ -7585,7 +7584,7 @@
         <v>2.6221999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" s="112">
         <v>-6.1304999999999998E-2</v>
       </c>
@@ -7698,7 +7697,7 @@
         <v>2.1964000000000001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37">
       <c r="A6" s="112">
         <v>-5.5215E-2</v>
       </c>
@@ -7811,7 +7810,7 @@
         <v>1.8523999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" s="112">
         <v>-5.0608E-2</v>
       </c>
@@ -7924,7 +7923,7 @@
         <v>1.6164999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" s="112">
         <v>-4.7326E-2</v>
       </c>
@@ -8037,7 +8036,7 @@
         <v>1.4739E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" s="112">
         <v>-4.3756999999999997E-2</v>
       </c>
@@ -8150,7 +8149,7 @@
         <v>1.3438E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" s="112">
         <v>-3.9752000000000003E-2</v>
       </c>
@@ -8263,7 +8262,7 @@
         <v>1.2238000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" s="112">
         <v>-3.6818999999999998E-2</v>
       </c>
@@ -8376,7 +8375,7 @@
         <v>1.142E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" s="112">
         <v>-3.4412999999999999E-2</v>
       </c>
@@ -8489,7 +8488,7 @@
         <v>1.0888999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" s="112">
         <v>-3.1092000000000002E-2</v>
       </c>
@@ -8602,7 +8601,7 @@
         <v>1.0203E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" s="112">
         <v>-2.8393000000000002E-2</v>
       </c>
@@ -8715,7 +8714,7 @@
         <v>9.6659999999999992E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" s="112">
         <v>-2.5759000000000001E-2</v>
       </c>
@@ -8828,7 +8827,7 @@
         <v>9.2280000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" s="112">
         <v>-2.3243E-2</v>
       </c>
@@ -8941,7 +8940,7 @@
         <v>8.7810000000000006E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" s="112">
         <v>-2.1659000000000001E-2</v>
       </c>
@@ -9054,7 +9053,7 @@
         <v>8.4130000000000003E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" s="112">
         <v>-2.0065E-2</v>
       </c>
@@ -9167,7 +9166,7 @@
         <v>8.1679999999999999E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" s="112">
         <v>-1.8825999999999999E-2</v>
       </c>
@@ -9280,7 +9279,7 @@
         <v>7.8960000000000002E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" s="112">
         <v>-1.8134000000000001E-2</v>
       </c>
@@ -9393,7 +9392,7 @@
         <v>7.6779999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" s="112">
         <v>-1.721E-2</v>
       </c>
@@ -9506,7 +9505,7 @@
         <v>7.476E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" s="112">
         <v>-1.6492E-2</v>
       </c>
@@ -9619,7 +9618,7 @@
         <v>7.2880000000000002E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
       <c r="A23" s="112">
         <v>-1.5685999999999999E-2</v>
       </c>
@@ -9732,7 +9731,7 @@
         <v>7.1419999999999999E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37">
       <c r="A24" s="112">
         <v>-1.5132E-2</v>
       </c>
@@ -9845,7 +9844,7 @@
         <v>6.9940000000000002E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" s="112">
         <v>-1.4701000000000001E-2</v>
       </c>
@@ -9958,7 +9957,7 @@
         <v>6.9109999999999996E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" s="112">
         <v>-1.4076999999999999E-2</v>
       </c>
@@ -10071,7 +10070,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" s="112">
         <v>-1.3455999999999999E-2</v>
       </c>
@@ -10184,7 +10183,7 @@
         <v>6.7759999999999999E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37">
       <c r="A28" s="112">
         <v>-1.311E-2</v>
       </c>
@@ -10297,7 +10296,7 @@
         <v>6.711E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" s="112">
         <v>-1.2841999999999999E-2</v>
       </c>
@@ -10410,7 +10409,7 @@
         <v>6.6509999999999998E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" s="112">
         <v>-1.2413E-2</v>
       </c>
@@ -10523,7 +10522,7 @@
         <v>6.6119999999999998E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37">
       <c r="A31" s="112">
         <v>-1.2324E-2</v>
       </c>
@@ -10636,7 +10635,7 @@
         <v>6.5160000000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37">
       <c r="A32" s="112">
         <v>-1.2546E-2</v>
       </c>
@@ -10749,7 +10748,7 @@
         <v>6.4590000000000003E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37">
       <c r="A33" s="112">
         <v>-1.2839E-2</v>
       </c>
@@ -10862,7 +10861,7 @@
         <v>6.3359999999999996E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37">
       <c r="A34" s="112">
         <v>-1.2834E-2</v>
       </c>
@@ -10975,7 +10974,7 @@
         <v>6.1939999999999999E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37">
       <c r="A35" s="112">
         <v>-1.2711E-2</v>
       </c>
@@ -11088,7 +11087,7 @@
         <v>6.0239999999999998E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37">
       <c r="A36" s="112">
         <v>-1.2652999999999999E-2</v>
       </c>
@@ -11201,7 +11200,7 @@
         <v>5.7939999999999997E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37">
       <c r="A37" s="112">
         <v>-1.2411E-2</v>
       </c>
@@ -11314,7 +11313,7 @@
         <v>5.5750000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37">
       <c r="A38" s="112">
         <v>-1.2128999999999999E-2</v>
       </c>
@@ -11427,7 +11426,7 @@
         <v>5.3619999999999996E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37">
       <c r="A39" s="112">
         <v>-1.1508000000000001E-2</v>
       </c>
@@ -11540,7 +11539,7 @@
         <v>5.0720000000000001E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37">
       <c r="A40" s="112">
         <v>-1.1006999999999999E-2</v>
       </c>
@@ -11653,7 +11652,7 @@
         <v>4.8349999999999999E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37">
       <c r="A41" s="112">
         <v>-1.0260999999999999E-2</v>
       </c>
@@ -11766,7 +11765,7 @@
         <v>4.5909999999999996E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37">
       <c r="A42" s="112">
         <v>-9.6329999999999992E-3</v>
       </c>
@@ -11879,7 +11878,7 @@
         <v>4.2880000000000001E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37">
       <c r="A43" s="112">
         <v>-6.2719999999999998E-3</v>
       </c>
@@ -11992,7 +11991,7 @@
         <v>3.4619999999999998E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37">
       <c r="A44" s="112">
         <v>-6.1310000000000002E-3</v>
       </c>
@@ -12105,7 +12104,7 @@
         <v>2.954E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37">
       <c r="A45" s="112">
         <v>-6.0780000000000001E-3</v>
       </c>
@@ -12218,7 +12217,7 @@
         <v>2.5560000000000001E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37">
       <c r="A46" s="112">
         <v>-6.0359999999999997E-3</v>
       </c>
@@ -12331,7 +12330,7 @@
         <v>2.1900000000000001E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37">
       <c r="A47" s="112">
         <v>-6.0520000000000001E-3</v>
       </c>
@@ -12444,7 +12443,7 @@
         <v>1.949E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37">
       <c r="A48" s="112">
         <v>-6.1879999999999999E-3</v>
       </c>
@@ -12557,7 +12556,7 @@
         <v>1.7060000000000001E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37">
       <c r="A49" s="112">
         <v>-6.0670000000000003E-3</v>
       </c>
@@ -12670,7 +12669,7 @@
         <v>1.601E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37">
       <c r="A50" s="112">
         <v>-6.2570000000000004E-3</v>
       </c>
@@ -12783,7 +12782,7 @@
         <v>1.523E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37">
       <c r="A51" s="112">
         <v>-6.3619999999999996E-3</v>
       </c>
@@ -12896,7 +12895,7 @@
         <v>1.4580000000000001E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37">
       <c r="A52" s="112">
         <v>-6.1390000000000004E-3</v>
       </c>
@@ -13009,7 +13008,7 @@
         <v>1.526E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37">
       <c r="A53" s="112">
         <v>-6.3169999999999997E-3</v>
       </c>
@@ -13122,7 +13121,7 @@
         <v>1.604E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37">
       <c r="A54" s="112">
         <v>-6.2379999999999996E-3</v>
       </c>
@@ -13235,7 +13234,7 @@
         <v>1.6559999999999999E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37">
       <c r="A55" s="112">
         <v>-6.2310000000000004E-3</v>
       </c>
@@ -13348,7 +13347,7 @@
         <v>1.787E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37">
       <c r="A56" s="112">
         <v>-6.3379999999999999E-3</v>
       </c>
@@ -13461,7 +13460,7 @@
         <v>1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37">
       <c r="A57" s="112">
         <v>-6.2969999999999996E-3</v>
       </c>
@@ -13574,7 +13573,7 @@
         <v>1.952E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37">
       <c r="A58" s="112">
         <v>-6.1679999999999999E-3</v>
       </c>
@@ -13687,7 +13686,7 @@
         <v>2.1189999999999998E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37">
       <c r="A59" s="112">
         <v>-6.3819999999999997E-3</v>
       </c>
@@ -13800,7 +13799,7 @@
         <v>2.186E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37">
       <c r="A60" s="112">
         <v>-6.4989999999999996E-3</v>
       </c>
@@ -13913,7 +13912,7 @@
         <v>2.313E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37">
       <c r="A61" s="112">
         <v>-6.5680000000000001E-3</v>
       </c>
@@ -14026,7 +14025,7 @@
         <v>2.4260000000000002E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37">
       <c r="A62" s="112">
         <v>-6.5700000000000003E-3</v>
       </c>
@@ -14139,7 +14138,7 @@
         <v>2.539E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37">
       <c r="A63" s="112">
         <v>-6.4590000000000003E-3</v>
       </c>
@@ -14252,7 +14251,7 @@
         <v>2.5969999999999999E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37">
       <c r="A64" s="112">
         <v>-6.4390000000000003E-3</v>
       </c>
@@ -14365,7 +14364,7 @@
         <v>2.7750000000000001E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37">
       <c r="A65" s="112">
         <v>-6.7149999999999996E-3</v>
       </c>
@@ -14478,7 +14477,7 @@
         <v>2.921E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37">
       <c r="A66" s="112">
         <v>-6.7669999999999996E-3</v>
       </c>
@@ -14591,7 +14590,7 @@
         <v>3.0200000000000001E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37">
       <c r="A67" s="112">
         <v>-6.8799999999999998E-3</v>
       </c>
@@ -14704,7 +14703,7 @@
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37">
       <c r="A68" s="112">
         <v>-6.6959999999999997E-3</v>
       </c>
@@ -14817,7 +14816,7 @@
         <v>3.3240000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37">
       <c r="A69" s="112">
         <v>-6.7229999999999998E-3</v>
       </c>
@@ -14930,7 +14929,7 @@
         <v>3.3570000000000002E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37">
       <c r="A70" s="112">
         <v>-6.3749999999999996E-3</v>
       </c>
@@ -15043,7 +15042,7 @@
         <v>3.4380000000000001E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37">
       <c r="A71" s="112">
         <v>-6.6249999999999998E-3</v>
       </c>
@@ -15156,7 +15155,7 @@
         <v>3.4480000000000001E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37">
       <c r="A72" s="112">
         <v>-6.1219999999999998E-3</v>
       </c>
@@ -15269,7 +15268,7 @@
         <v>3.444E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37">
       <c r="A73" s="112">
         <v>-5.9829999999999996E-3</v>
       </c>
@@ -15382,7 +15381,7 @@
         <v>3.4889999999999999E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37">
       <c r="A74" s="112">
         <v>-6.0089999999999996E-3</v>
       </c>
@@ -15495,7 +15494,7 @@
         <v>3.3140000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37">
       <c r="A75" s="112">
         <v>-5.5570000000000003E-3</v>
       </c>
@@ -15608,7 +15607,7 @@
         <v>3.3110000000000001E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37">
       <c r="A76" s="112">
         <v>-5.7099999999999998E-3</v>
       </c>
@@ -15721,7 +15720,7 @@
         <v>3.2759999999999998E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37">
       <c r="A77" s="112">
         <v>-5.7060000000000001E-3</v>
       </c>
@@ -15834,7 +15833,7 @@
         <v>3.1220000000000002E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37">
       <c r="A78" s="112">
         <v>-5.5230000000000001E-3</v>
       </c>
@@ -15947,7 +15946,7 @@
         <v>2.993E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37">
       <c r="A79" s="112">
         <v>-5.4010000000000004E-3</v>
       </c>
@@ -16060,7 +16059,7 @@
         <v>3.0300000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37">
       <c r="A80" s="112">
         <v>-5.8849999999999996E-3</v>
       </c>
@@ -16173,7 +16172,7 @@
         <v>3.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37">
       <c r="A81" s="112">
         <v>-5.5620000000000001E-3</v>
       </c>
@@ -16286,7 +16285,7 @@
         <v>3.0230000000000001E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37">
       <c r="A82" s="112">
         <v>-5.6230000000000004E-3</v>
       </c>
@@ -16399,7 +16398,7 @@
         <v>2.9949999999999998E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37">
       <c r="A83" s="112">
         <v>-5.594E-3</v>
       </c>
@@ -16530,12 +16529,12 @@
       <selection activeCell="AK83" sqref="AK83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="112"/>
+    <col min="1" max="16384" width="8.83203125" style="112"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37">
       <c r="A1" s="112">
         <v>1.7951000000000002E-2</v>
       </c>
@@ -16648,7 +16647,7 @@
         <v>-1.6435000000000002E-2</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37">
       <c r="A2" s="112">
         <v>1.2437E-2</v>
       </c>
@@ -16761,7 +16760,7 @@
         <v>-1.3527000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37">
       <c r="A3" s="112">
         <v>5.5900000000000004E-3</v>
       </c>
@@ -16874,7 +16873,7 @@
         <v>-1.1609E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37">
       <c r="A4" s="112">
         <v>2.441E-3</v>
       </c>
@@ -16987,7 +16986,7 @@
         <v>-9.3799999999999994E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37">
       <c r="A5" s="112">
         <v>3.0769999999999999E-3</v>
       </c>
@@ -17100,7 +17099,7 @@
         <v>-7.8279999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37">
       <c r="A6" s="112">
         <v>-1.7229999999999999E-3</v>
       </c>
@@ -17213,7 +17212,7 @@
         <v>-7.2960000000000004E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37">
       <c r="A7" s="112">
         <v>-1.639E-3</v>
       </c>
@@ -17326,7 +17325,7 @@
         <v>-5.6899999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37">
       <c r="A8" s="112">
         <v>-3.9490000000000003E-3</v>
       </c>
@@ -17439,7 +17438,7 @@
         <v>-5.0899999999999999E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37">
       <c r="A9" s="112">
         <v>-5.091E-3</v>
       </c>
@@ -17552,7 +17551,7 @@
         <v>-4.3169999999999997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37">
       <c r="A10" s="112">
         <v>-6.2509999999999996E-3</v>
       </c>
@@ -17665,7 +17664,7 @@
         <v>-3.8920000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37">
       <c r="A11" s="112">
         <v>-7.6689999999999996E-3</v>
       </c>
@@ -17778,7 +17777,7 @@
         <v>-3.3760000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37">
       <c r="A12" s="112">
         <v>-7.5690000000000002E-3</v>
       </c>
@@ -17891,7 +17890,7 @@
         <v>-2.9299999999999999E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37">
       <c r="A13" s="112">
         <v>-7.8449999999999995E-3</v>
       </c>
@@ -18004,7 +18003,7 @@
         <v>-2.6180000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37">
       <c r="A14" s="112">
         <v>-8.1080000000000006E-3</v>
       </c>
@@ -18117,7 +18116,7 @@
         <v>-2.1870000000000001E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37">
       <c r="A15" s="112">
         <v>-8.1810000000000008E-3</v>
       </c>
@@ -18230,7 +18229,7 @@
         <v>-2.0899999999999998E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37">
       <c r="A16" s="112">
         <v>-7.0410000000000004E-3</v>
       </c>
@@ -18343,7 +18342,7 @@
         <v>-1.684E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:37">
       <c r="A17" s="112">
         <v>-7.5420000000000001E-3</v>
       </c>
@@ -18456,7 +18455,7 @@
         <v>-1.601E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37">
       <c r="A18" s="112">
         <v>-6.7739999999999996E-3</v>
       </c>
@@ -18569,7 +18568,7 @@
         <v>-1.341E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37">
       <c r="A19" s="112">
         <v>-5.7710000000000001E-3</v>
       </c>
@@ -18682,7 +18681,7 @@
         <v>-1.013E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:37">
       <c r="A20" s="112">
         <v>-6.5979999999999997E-3</v>
       </c>
@@ -18795,7 +18794,7 @@
         <v>-1.0449999999999999E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:37">
       <c r="A21" s="112">
         <v>-5.731E-3</v>
       </c>
@@ -18908,7 +18907,7 @@
         <v>-7.9299999999999998E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:37">
       <c r="A22" s="112">
         <v>-5.2379999999999996E-3</v>
       </c>
@@ -19021,7 +19020,7 @@
         <v>-5.4199999999999995E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:37">
       <c r="A23" s="112">
         <v>-5.9519999999999998E-3</v>
       </c>
@@ -19134,7 +19133,7 @@
         <v>-6.0300000000000002E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:37">
       <c r="A24" s="112">
         <v>-5.2240000000000003E-3</v>
       </c>
@@ -19247,7 +19246,7 @@
         <v>-5.0199999999999995E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:37">
       <c r="A25" s="112">
         <v>-4.816E-3</v>
       </c>
@@ -19360,7 +19359,7 @@
         <v>-2.8699999999999998E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:37">
       <c r="A26" s="112">
         <v>-5.1489999999999999E-3</v>
       </c>
@@ -19473,7 +19472,7 @@
         <v>-2.9300000000000002E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:37">
       <c r="A27" s="112">
         <v>-4.5799999999999999E-3</v>
       </c>
@@ -19586,7 +19585,7 @@
         <v>-1.8799999999999999E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:37">
       <c r="A28" s="112">
         <v>-3.9309999999999996E-3</v>
       </c>
@@ -19699,7 +19698,7 @@
         <v>-8.2999999999999998E-5</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:37">
       <c r="A29" s="112">
         <v>-4.3629999999999997E-3</v>
       </c>
@@ -19812,7 +19811,7 @@
         <v>-4.1999999999999998E-5</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:37">
       <c r="A30" s="112">
         <v>-3.0850000000000001E-3</v>
       </c>
@@ -19925,7 +19924,7 @@
         <v>1.2999999999999999E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:37">
       <c r="A31" s="112">
         <v>-3.1389999999999999E-3</v>
       </c>
@@ -20038,7 +20037,7 @@
         <v>2.1499999999999999E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:37">
       <c r="A32" s="112">
         <v>-3.1210000000000001E-3</v>
       </c>
@@ -20151,7 +20150,7 @@
         <v>1.9100000000000001E-4</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:37">
       <c r="A33" s="112">
         <v>-2.4740000000000001E-3</v>
       </c>
@@ -20264,7 +20263,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:37">
       <c r="A34" s="112">
         <v>-2.5569999999999998E-3</v>
       </c>
@@ -20377,7 +20376,7 @@
         <v>4.2299999999999998E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:37">
       <c r="A35" s="112">
         <v>-2.9510000000000001E-3</v>
       </c>
@@ -20490,7 +20489,7 @@
         <v>3.68E-4</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:37">
       <c r="A36" s="112">
         <v>-2.545E-3</v>
       </c>
@@ -20603,7 +20602,7 @@
         <v>4.57E-4</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:37">
       <c r="A37" s="112">
         <v>-2.5179999999999998E-3</v>
       </c>
@@ -20716,7 +20715,7 @@
         <v>4.0099999999999999E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:37">
       <c r="A38" s="112">
         <v>-2.8119999999999998E-3</v>
       </c>
@@ -20829,7 +20828,7 @@
         <v>3.6900000000000002E-4</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:37">
       <c r="A39" s="112">
         <v>-2.5339999999999998E-3</v>
       </c>
@@ -20942,7 +20941,7 @@
         <v>3.57E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:37">
       <c r="A40" s="112">
         <v>-2.5709999999999999E-3</v>
       </c>
@@ -21055,7 +21054,7 @@
         <v>2.13E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:37">
       <c r="A41" s="112">
         <v>-1.9480000000000001E-3</v>
       </c>
@@ -21168,7 +21167,7 @@
         <v>5.8E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:37">
       <c r="A42" s="112">
         <v>-2.0049999999999998E-3</v>
       </c>
@@ -21281,7 +21280,7 @@
         <v>-7.4999999999999993E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:37">
       <c r="A43" s="112">
         <v>-1.8489999999999999E-3</v>
       </c>
@@ -21394,7 +21393,7 @@
         <v>-3.48E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:37">
       <c r="A44" s="112">
         <v>-1.8420000000000001E-3</v>
       </c>
@@ -21507,7 +21506,7 @@
         <v>-4.9799999999999996E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:37">
       <c r="A45" s="112">
         <v>-1.792E-3</v>
       </c>
@@ -21620,7 +21619,7 @@
         <v>-8.0900000000000004E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:37">
       <c r="A46" s="112">
         <v>-1.946E-3</v>
       </c>
@@ -21733,7 +21732,7 @@
         <v>-9.3700000000000001E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:37">
       <c r="A47" s="112">
         <v>-1.89E-3</v>
       </c>
@@ -21846,7 +21845,7 @@
         <v>-1.034E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:37">
       <c r="A48" s="112">
         <v>-1.9959999999999999E-3</v>
       </c>
@@ -21959,7 +21958,7 @@
         <v>-1.294E-3</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:37">
       <c r="A49" s="112">
         <v>-2.1489999999999999E-3</v>
       </c>
@@ -22072,7 +22071,7 @@
         <v>-1.457E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:37">
       <c r="A50" s="112">
         <v>-1.9120000000000001E-3</v>
       </c>
@@ -22185,7 +22184,7 @@
         <v>-1.523E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:37">
       <c r="A51" s="112">
         <v>-1.7960000000000001E-3</v>
       </c>
@@ -22298,7 +22297,7 @@
         <v>-1.642E-3</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:37">
       <c r="A52" s="112">
         <v>-1.7769999999999999E-3</v>
       </c>
@@ -22411,7 +22410,7 @@
         <v>-1.5770000000000001E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:37">
       <c r="A53" s="112">
         <v>-1.918E-3</v>
       </c>
@@ -22524,7 +22523,7 @@
         <v>-1.8879999999999999E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:37">
       <c r="A54" s="112">
         <v>-1.3630000000000001E-3</v>
       </c>
@@ -22637,7 +22636,7 @@
         <v>-1.784E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:37">
       <c r="A55" s="112">
         <v>-1.34E-3</v>
       </c>
@@ -22750,7 +22749,7 @@
         <v>-1.835E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:37">
       <c r="A56" s="112">
         <v>-1.142E-3</v>
       </c>
@@ -22863,7 +22862,7 @@
         <v>-1.885E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:37">
       <c r="A57" s="112">
         <v>-7.5900000000000002E-4</v>
       </c>
@@ -22976,7 +22975,7 @@
         <v>-1.946E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:37">
       <c r="A58" s="112">
         <v>-6.1399999999999996E-4</v>
       </c>
@@ -23089,7 +23088,7 @@
         <v>-1.946E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:37">
       <c r="A59" s="112">
         <v>-4.7800000000000002E-4</v>
       </c>
@@ -23202,7 +23201,7 @@
         <v>-1.902E-3</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:37">
       <c r="A60" s="112">
         <v>-8.1000000000000004E-5</v>
       </c>
@@ -23315,7 +23314,7 @@
         <v>-1.9620000000000002E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:37">
       <c r="A61" s="112">
         <v>-6.3E-5</v>
       </c>
@@ -23428,7 +23427,7 @@
         <v>-1.8990000000000001E-3</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:37">
       <c r="A62" s="112">
         <v>-1.2999999999999999E-5</v>
       </c>
@@ -23541,7 +23540,7 @@
         <v>-1.882E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:37">
       <c r="A63" s="112">
         <v>2.02E-4</v>
       </c>
@@ -23654,7 +23653,7 @@
         <v>-1.8400000000000001E-3</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:37">
       <c r="A64" s="112">
         <v>-1.2999999999999999E-4</v>
       </c>
@@ -23767,7 +23766,7 @@
         <v>-1.867E-3</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:37">
       <c r="A65" s="112">
         <v>-3.4200000000000002E-4</v>
       </c>
@@ -23880,7 +23879,7 @@
         <v>-1.8309999999999999E-3</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:37">
       <c r="A66" s="112">
         <v>-4.3999999999999999E-5</v>
       </c>
@@ -23993,7 +23992,7 @@
         <v>-1.622E-3</v>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:37">
       <c r="A67" s="112">
         <v>9.9999999999999995E-7</v>
       </c>
@@ -24106,7 +24105,7 @@
         <v>-1.689E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:37">
       <c r="A68" s="112">
         <v>-1.7100000000000001E-4</v>
       </c>
@@ -24219,7 +24218,7 @@
         <v>-1.5870000000000001E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:37">
       <c r="A69" s="112">
         <v>1.15E-4</v>
       </c>
@@ -24332,7 +24331,7 @@
         <v>-1.482E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:37">
       <c r="A70" s="112">
         <v>1.02E-4</v>
       </c>
@@ -24445,7 +24444,7 @@
         <v>-1.3519999999999999E-3</v>
       </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:37">
       <c r="A71" s="112">
         <v>9.0000000000000006E-5</v>
       </c>
@@ -24558,7 +24557,7 @@
         <v>-1.2049999999999999E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:37">
       <c r="A72" s="112">
         <v>7.0699999999999995E-4</v>
       </c>
@@ -24671,7 +24670,7 @@
         <v>-1.191E-3</v>
       </c>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:37">
       <c r="A73" s="112">
         <v>4.6200000000000001E-4</v>
       </c>
@@ -24784,7 +24783,7 @@
         <v>-1.1100000000000001E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:37">
       <c r="A74" s="112">
         <v>1.178E-3</v>
       </c>
@@ -24897,7 +24896,7 @@
         <v>-1.1820000000000001E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:37">
       <c r="A75" s="112">
         <v>1.0859999999999999E-3</v>
       </c>
@@ -25010,7 +25009,7 @@
         <v>-1.0939999999999999E-3</v>
       </c>
     </row>
-    <row r="76" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:37">
       <c r="A76" s="112">
         <v>1.1479999999999999E-3</v>
       </c>
@@ -25123,7 +25122,7 @@
         <v>-1.0560000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:37">
       <c r="A77" s="112">
         <v>1.6659999999999999E-3</v>
       </c>
@@ -25236,7 +25235,7 @@
         <v>-1.0889999999999999E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:37">
       <c r="A78" s="112">
         <v>1.645E-3</v>
       </c>
@@ -25349,7 +25348,7 @@
         <v>-1.2639999999999999E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:37">
       <c r="A79" s="112">
         <v>1.446E-3</v>
       </c>
@@ -25462,7 +25461,7 @@
         <v>-1.175E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:37">
       <c r="A80" s="112">
         <v>1.7979999999999999E-3</v>
       </c>
@@ -25575,7 +25574,7 @@
         <v>-1.2800000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:37">
       <c r="A81" s="112">
         <v>1.81E-3</v>
       </c>
@@ -25688,7 +25687,7 @@
         <v>-1.4220000000000001E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:37">
       <c r="A82" s="112">
         <v>1.4289999999999999E-3</v>
       </c>
@@ -25801,7 +25800,7 @@
         <v>-1.397E-3</v>
       </c>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:37">
       <c r="A83" s="112">
         <v>2.15E-3</v>
       </c>

</xml_diff>